<commit_message>
IR Module - Common Methods.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="7" activeTab="11"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="UpdatedIndividuals" sheetId="14" r:id="rId11"/>
     <sheet name="AddVitals" sheetId="11" r:id="rId12"/>
     <sheet name="EditVitals" sheetId="13" r:id="rId13"/>
+    <sheet name="Incident Reports" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="185">
   <si>
     <t>Environment Name</t>
   </si>
@@ -729,6 +730,72 @@
   <si>
     <t>ABCD</t>
   </si>
+  <si>
+    <t>Individual's Details</t>
+  </si>
+  <si>
+    <t>Event Date &amp; Time</t>
+  </si>
+  <si>
+    <t>What caused the fall?</t>
+  </si>
+  <si>
+    <t>Injury Description</t>
+  </si>
+  <si>
+    <t>Was Individual injured?</t>
+  </si>
+  <si>
+    <t>Injury Site - Front View</t>
+  </si>
+  <si>
+    <t>Injury Site - Back View</t>
+  </si>
+  <si>
+    <t>Treatment Received</t>
+  </si>
+  <si>
+    <t>Future Treatment</t>
+  </si>
+  <si>
+    <t>Injury Type</t>
+  </si>
+  <si>
+    <t>Injury Color</t>
+  </si>
+  <si>
+    <t>How severe was the injury?</t>
+  </si>
+  <si>
+    <t>Person Notified</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Notification Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Notified By</t>
+  </si>
+  <si>
+    <t>Notification Method</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Fore Head , Face , Right Shoulder , Left Shoulder , Right Arm , Left Arm ,  Chest , Abdomen , Right Wrist , Left Wrist , Right Knee , Left Knee , Right Foot , Left Foot</t>
+  </si>
+  <si>
+    <t>Head , Face , Left Shoulder , Right Shoulder , Left Arm , Right Arm ,  Back , Hip , Left Wrist , Right Wrist , Left Knee , Right Knee , Left Foot , Right Foot</t>
+  </si>
+  <si>
+    <t>Abrasion , Bleeding , Bruise , Scratch</t>
+  </si>
 </sst>
 </file>
 
@@ -740,13 +807,34 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Comic Sans MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00151D"/>
+      <name val="Comic Sans MS"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -778,13 +866,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF6A3E3E"/>
-      <name val="Comic Sans MS"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Comic Sans MS"/>
       <charset val="134"/>
     </font>
@@ -1418,195 +1499,201 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1614,43 +1701,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1985,34 +2072,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="51" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2040,7 +2127,7 @@
   <cols>
     <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
     <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
-    <col min="7" max="7" width="27.6363636363636" style="11" customWidth="1"/>
+    <col min="7" max="7" width="27.6363636363636" style="16" customWidth="1"/>
     <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
     <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
     <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
@@ -2051,201 +2138,201 @@
     <col min="28" max="16383" width="10.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="17" spans="1:27">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="16" customFormat="1" ht="17" spans="1:27">
+      <c r="A1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" ht="17.5" spans="1:27">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="51" t="s">
+      <c r="U2" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="52" t="s">
+      <c r="V2" s="5"/>
+      <c r="W2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="52" t="s">
+      <c r="X2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="52" t="s">
+      <c r="Y2" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="Z2" s="52" t="s">
+      <c r="Z2" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="3" spans="5:21">
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="5:7">
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="20"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="20"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="20"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -2266,7 +2353,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="24">
         <v>6</v>
       </c>
       <c r="H8">
@@ -2331,130 +2418,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="20"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="20"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="20"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="20"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="20"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="20"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="20"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="20"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="20"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="20"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="20"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="20"/>
+      <c r="G20" s="24"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="20"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="20"/>
+      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="20"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="20"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="20"/>
+      <c r="G25" s="24"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="20"/>
+      <c r="G26" s="24"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="20"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="20"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="20"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="20"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="20"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="20"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="20"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="20"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="20"/>
+      <c r="G35" s="24"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="20"/>
+      <c r="G36" s="24"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="20"/>
+      <c r="G37" s="24"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="20"/>
+      <c r="G38" s="24"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="20"/>
+      <c r="G39" s="24"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="20"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="20"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="20"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="20"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="20"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="20"/>
+      <c r="G45" s="24"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="20"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="20"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="20"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="20"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="20"/>
+      <c r="G50" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2478,10 +2565,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2496,7 +2583,7 @@
   <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2513,55 +2600,55 @@
     <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="1" spans="1:8">
+      <c r="A1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="58" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2592,18 +2679,18 @@
       </c>
     </row>
     <row r="6" ht="17.5" spans="7:8">
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="13" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="13" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2635,66 +2722,66 @@
     <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="1" spans="1:9">
+      <c r="A1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="14" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="3" spans="9:9">
-      <c r="I3" s="4"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
@@ -2723,22 +2810,140 @@
       </c>
     </row>
     <row r="6" ht="17.5" spans="7:8">
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="13" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="13" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="2" width="20.0909090909091" customWidth="1"/>
+    <col min="3" max="3" width="24.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="20.0909090909091" customWidth="1"/>
+    <col min="5" max="5" width="24.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="25.5454545454545" customWidth="1"/>
+    <col min="7" max="7" width="25.2727272727273" customWidth="1"/>
+    <col min="8" max="9" width="20.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="30.6363636363636" customWidth="1"/>
+    <col min="11" max="11" width="18.5454545454545" customWidth="1"/>
+    <col min="12" max="16384" width="20.0909090909091" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="17" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" ht="87" spans="1:18">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E$1:E$1048576">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2761,24 +2966,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2806,57 +3011,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="36" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="36" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="36" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2881,75 +3086,75 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.6363636363636" style="26" customWidth="1"/>
-    <col min="2" max="2" width="28.7272727272727" style="26" customWidth="1"/>
-    <col min="3" max="5" width="12.6363636363636" style="26" customWidth="1"/>
+    <col min="1" max="1" width="12.6363636363636" style="30" customWidth="1"/>
+    <col min="2" max="2" width="28.7272727272727" style="30" customWidth="1"/>
+    <col min="3" max="5" width="12.6363636363636" style="30" customWidth="1"/>
     <col min="6" max="6" width="20.2727272727273" customWidth="1"/>
     <col min="7" max="7" width="16.8181818181818" customWidth="1"/>
     <col min="8" max="16381" width="12.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="33" customFormat="1" ht="19.5" spans="1:7">
-      <c r="A1" s="27" t="s">
+    <row r="1" s="37" customFormat="1" ht="19.5" spans="1:7">
+      <c r="A1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="7:7">
-      <c r="G3" s="4"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="26">
+      <c r="A6" s="30">
         <v>0</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="30">
         <v>1</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="30">
         <v>2</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="30">
         <v>3</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="30">
         <v>4</v>
       </c>
       <c r="F6">
@@ -2978,62 +3183,62 @@
   <cols>
     <col min="1" max="1" width="21.7272727272727" customWidth="1"/>
     <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="12.9090909090909" style="26" customWidth="1"/>
+    <col min="3" max="5" width="12.9090909090909" style="30" customWidth="1"/>
     <col min="6" max="6" width="30.9090909090909" customWidth="1"/>
     <col min="7" max="7" width="22.2727272727273" customWidth="1"/>
     <col min="8" max="16379" width="12.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="26"/>
-      <c r="F3" s="32" t="s">
+      <c r="B3" s="30"/>
+      <c r="F3" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
@@ -3042,13 +3247,13 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="30">
         <v>2</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="30">
         <v>3</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="30">
         <v>4</v>
       </c>
       <c r="F10">
@@ -3079,7 +3284,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3105,10 +3310,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="29" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3131,7 +3336,7 @@
   <cols>
     <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
     <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
-    <col min="7" max="7" width="27.6363636363636" style="11" customWidth="1"/>
+    <col min="7" max="7" width="27.6363636363636" style="16" customWidth="1"/>
     <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
     <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
     <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
@@ -3142,201 +3347,201 @@
     <col min="28" max="16384" width="10.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="17" spans="1:27">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="16" customFormat="1" ht="17" spans="1:27">
+      <c r="A1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="51" t="s">
+      <c r="U2" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="52" t="s">
+      <c r="V2" s="5"/>
+      <c r="W2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="52" t="s">
+      <c r="X2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="52" t="s">
+      <c r="Y2" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="Z2" s="52" t="s">
+      <c r="Z2" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="5:21">
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="5:7">
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="20"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="20"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="20"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -3357,7 +3562,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="24">
         <v>6</v>
       </c>
       <c r="H8">
@@ -3422,130 +3627,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="20"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="20"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="20"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="20"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="20"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="20"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="20"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="20"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="20"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="20"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="20"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="20"/>
+      <c r="G20" s="24"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="20"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="20"/>
+      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="20"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="20"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="20"/>
+      <c r="G25" s="24"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="20"/>
+      <c r="G26" s="24"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="20"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="20"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="20"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="20"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="20"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="20"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="20"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="20"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="20"/>
+      <c r="G35" s="24"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="20"/>
+      <c r="G36" s="24"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="20"/>
+      <c r="G37" s="24"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="20"/>
+      <c r="G38" s="24"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="20"/>
+      <c r="G39" s="24"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="20"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="20"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="20"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="20"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="20"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="20"/>
+      <c r="G45" s="24"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="20"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="20"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="20"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="20"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="20"/>
+      <c r="G50" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3570,13 +3775,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IR flow step definitions for staff user added.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="9" activeTab="13"/>
+    <workbookView windowWidth="19635" windowHeight="7200" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -801,11 +801,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -1487,16 +1488,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1629,7 +1630,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1639,6 +1640,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1661,7 +1665,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1730,7 +1734,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
@@ -2065,41 +2069,41 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="29.0909090909091" customWidth="1"/>
+    <col min="1" max="1" width="17.3619047619048" customWidth="1"/>
+    <col min="2" max="2" width="29.0952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2123,38 +2127,38 @@
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.9047619047619" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
-    <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
-    <col min="7" max="7" width="27.6363636363636" style="16" customWidth="1"/>
-    <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
-    <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
-    <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
-    <col min="24" max="24" width="19.7272727272727" customWidth="1"/>
-    <col min="25" max="25" width="21.6363636363636" customWidth="1"/>
-    <col min="26" max="26" width="18.9090909090909" customWidth="1"/>
-    <col min="27" max="27" width="20.5454545454545" customWidth="1"/>
-    <col min="28" max="16383" width="10.9090909090909" customWidth="1"/>
+    <col min="1" max="5" width="21.3619047619048" customWidth="1"/>
+    <col min="6" max="6" width="11.4571428571429" customWidth="1"/>
+    <col min="7" max="7" width="27.6380952380952" style="17" customWidth="1"/>
+    <col min="8" max="8" width="9.36190476190476" customWidth="1"/>
+    <col min="9" max="22" width="21.3619047619048" customWidth="1"/>
+    <col min="23" max="23" width="16.4571428571429" customWidth="1"/>
+    <col min="24" max="24" width="19.7238095238095" customWidth="1"/>
+    <col min="25" max="25" width="21.6380952380952" customWidth="1"/>
+    <col min="26" max="26" width="18.9047619047619" customWidth="1"/>
+    <col min="27" max="27" width="20.5428571428571" customWidth="1"/>
+    <col min="28" max="16383" width="10.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="16" customFormat="1" ht="17" spans="1:27">
-      <c r="A1" s="17" t="s">
+    <row r="1" s="17" customFormat="1" ht="18" spans="1:27">
+      <c r="A1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>54</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2169,22 +2173,22 @@
       <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -2205,30 +2209,30 @@
       <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" ht="17.5" spans="1:27">
-      <c r="A2" s="19" t="s">
+    <row r="2" ht="17.25" spans="1:27">
+      <c r="A2" s="20" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>111</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2237,13 +2241,13 @@
       <c r="E2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>115</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -2252,13 +2256,13 @@
       <c r="J2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="27" t="s">
         <v>118</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -2273,29 +2277,29 @@
       <c r="Q2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="S2" s="29" t="s">
         <v>124</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="55" t="s">
+      <c r="U2" s="56" t="s">
         <v>96</v>
       </c>
       <c r="V2" s="5"/>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="56" t="s">
+      <c r="Y2" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="Z2" s="56" t="s">
+      <c r="Z2" s="57" t="s">
         <v>100</v>
       </c>
       <c r="AA2" s="5" t="s">
@@ -2306,13 +2310,13 @@
       <c r="E3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="28" t="s">
         <v>87</v>
       </c>
       <c r="U3" s="5" t="s">
@@ -2323,16 +2327,16 @@
       <c r="E4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="24"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="24"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -2353,7 +2357,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="25">
         <v>6</v>
       </c>
       <c r="H8">
@@ -2418,130 +2422,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="24"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="24"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="24"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="24"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="24"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="24"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="24"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="24"/>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="24"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="24"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="24"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="24"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="24"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="24"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="24"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="24"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="24"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="24"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="24"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="24"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="24"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="24"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="24"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="24"/>
+      <c r="G35" s="25"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="24"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="24"/>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="24"/>
+      <c r="G38" s="25"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="24"/>
+      <c r="G39" s="25"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="24"/>
+      <c r="G40" s="25"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="24"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="24"/>
+      <c r="G42" s="25"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="24"/>
+      <c r="G43" s="25"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="24"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="24"/>
+      <c r="G45" s="25"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="24"/>
+      <c r="G46" s="25"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="24"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="24"/>
+      <c r="G48" s="25"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="24"/>
+      <c r="G49" s="25"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="24"/>
+      <c r="G50" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2558,17 +2562,17 @@
       <selection activeCell="B16" sqref="A2:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="23.6363636363636" customWidth="1"/>
-    <col min="2" max="2" width="29.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="23.6380952380952" customWidth="1"/>
+    <col min="2" max="2" width="29.2761904761905" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2587,68 +2591,68 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="19.1809523809524" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="23.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="21.3636363636364" customWidth="1"/>
-    <col min="4" max="4" width="19.1818181818182" customWidth="1"/>
-    <col min="5" max="5" width="12.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="12.0909090909091" customWidth="1"/>
-    <col min="7" max="7" width="12.1818181818182" customWidth="1"/>
-    <col min="8" max="8" width="46.0909090909091" customWidth="1"/>
-    <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
+    <col min="1" max="1" width="13.2761904761905" customWidth="1"/>
+    <col min="2" max="2" width="23.2761904761905" customWidth="1"/>
+    <col min="3" max="3" width="21.3619047619048" customWidth="1"/>
+    <col min="4" max="4" width="19.1809523809524" customWidth="1"/>
+    <col min="5" max="5" width="12.6380952380952" customWidth="1"/>
+    <col min="6" max="6" width="12.0952380952381" customWidth="1"/>
+    <col min="7" max="7" width="12.1809523809524" customWidth="1"/>
+    <col min="8" max="8" width="46.0952380952381" customWidth="1"/>
+    <col min="9" max="16384" width="19.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="1" spans="1:8">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="8" customFormat="1" spans="1:8">
+      <c r="A1" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="56" t="s">
+    <row r="2" ht="15.75" spans="1:8">
+      <c r="A2" s="57" t="s">
         <v>141</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="59" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2678,19 +2682,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="17.5" spans="7:8">
-      <c r="G6" s="12" t="s">
+    <row r="6" ht="17.25" spans="7:8">
+      <c r="G6" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="7" ht="17.5" spans="7:8">
-      <c r="G7" s="12" t="s">
+    <row r="7" ht="17.25" spans="7:8">
+      <c r="G7" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2709,71 +2713,71 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="19.1809523809524" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="23.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="21.3636363636364" customWidth="1"/>
-    <col min="4" max="4" width="19.1818181818182" customWidth="1"/>
-    <col min="5" max="5" width="12.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="12.0909090909091" customWidth="1"/>
-    <col min="7" max="7" width="12.1818181818182" customWidth="1"/>
-    <col min="8" max="8" width="46.0909090909091" customWidth="1"/>
-    <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
+    <col min="1" max="1" width="13.2761904761905" customWidth="1"/>
+    <col min="2" max="2" width="23.2761904761905" customWidth="1"/>
+    <col min="3" max="3" width="21.3619047619048" customWidth="1"/>
+    <col min="4" max="4" width="19.1809523809524" customWidth="1"/>
+    <col min="5" max="5" width="12.6380952380952" customWidth="1"/>
+    <col min="6" max="6" width="12.0952380952381" customWidth="1"/>
+    <col min="7" max="7" width="12.1809523809524" customWidth="1"/>
+    <col min="8" max="8" width="46.0952380952381" customWidth="1"/>
+    <col min="9" max="16384" width="19.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="1" spans="1:9">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="8" customFormat="1" spans="1:9">
+      <c r="A1" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:9">
+    <row r="2" ht="15.75" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>154</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="60" t="s">
         <v>161</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -2809,19 +2813,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="17.5" spans="7:8">
-      <c r="G6" s="12" t="s">
+    <row r="6" ht="17.25" spans="7:8">
+      <c r="G6" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="7" ht="17.5" spans="7:8">
-      <c r="G7" s="12" t="s">
+    <row r="7" ht="17.25" spans="7:8">
+      <c r="G7" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2836,25 +2840,25 @@
   <sheetPr/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="20.0952380952381" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="2" width="20.0909090909091" customWidth="1"/>
-    <col min="3" max="3" width="24.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="20.0909090909091" customWidth="1"/>
-    <col min="5" max="5" width="24.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="25.5454545454545" customWidth="1"/>
-    <col min="7" max="7" width="25.2727272727273" customWidth="1"/>
-    <col min="8" max="9" width="20.0909090909091" customWidth="1"/>
-    <col min="10" max="10" width="30.6363636363636" customWidth="1"/>
-    <col min="11" max="11" width="18.5454545454545" customWidth="1"/>
-    <col min="12" max="16384" width="20.0909090909091" customWidth="1"/>
+    <col min="1" max="2" width="20.0952380952381" customWidth="1"/>
+    <col min="3" max="3" width="24.2761904761905" customWidth="1"/>
+    <col min="4" max="4" width="20.0952380952381" customWidth="1"/>
+    <col min="5" max="5" width="24.2761904761905" customWidth="1"/>
+    <col min="6" max="6" width="25.5428571428571" customWidth="1"/>
+    <col min="7" max="7" width="25.2761904761905" customWidth="1"/>
+    <col min="8" max="9" width="20.0952380952381" customWidth="1"/>
+    <col min="10" max="10" width="30.6380952380952" customWidth="1"/>
+    <col min="11" max="11" width="18.5428571428571" customWidth="1"/>
+    <col min="12" max="16384" width="20.0952380952381" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="17" spans="1:18">
+    <row r="1" s="1" customFormat="1" ht="18" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
@@ -2910,7 +2914,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" ht="87" spans="1:18">
+    <row r="2" ht="90" spans="1:18">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2926,7 +2930,7 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="7" t="s">
         <v>184</v>
       </c>
       <c r="K2" s="5"/>
@@ -2939,9 +2943,21 @@
       <c r="R2" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E$1:E$1048576">
       <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K$1:K$1048576">
+      <formula1>"Red,Green,Black,Brown"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
+      <formula1>"Light,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576">
+      <formula1>"Guardian,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R$1:R$1048576">
+      <formula1>"Phone Call,Email,Text Message"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2958,29 +2974,29 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="31.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="27.3636363636364" customWidth="1"/>
-    <col min="3" max="3" width="14.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="31.2761904761905" customWidth="1"/>
+    <col min="2" max="2" width="27.3619047619048" customWidth="1"/>
+    <col min="3" max="3" width="14.2761904761905" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="5"/>
@@ -3003,7 +3019,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
@@ -3011,57 +3027,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3084,56 +3100,56 @@
       <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.6363636363636" style="30" customWidth="1"/>
-    <col min="2" max="2" width="28.7272727272727" style="30" customWidth="1"/>
-    <col min="3" max="5" width="12.6363636363636" style="30" customWidth="1"/>
-    <col min="6" max="6" width="20.2727272727273" customWidth="1"/>
-    <col min="7" max="7" width="16.8181818181818" customWidth="1"/>
-    <col min="8" max="16381" width="12.6363636363636" customWidth="1"/>
+    <col min="1" max="1" width="12.6380952380952" style="31" customWidth="1"/>
+    <col min="2" max="2" width="28.7238095238095" style="31" customWidth="1"/>
+    <col min="3" max="5" width="12.6380952380952" style="31" customWidth="1"/>
+    <col min="6" max="6" width="20.2761904761905" customWidth="1"/>
+    <col min="7" max="7" width="16.8190476190476" customWidth="1"/>
+    <col min="8" max="16381" width="12.6380952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="37" customFormat="1" ht="19.5" spans="1:7">
-      <c r="A1" s="31" t="s">
+    <row r="1" s="38" customFormat="1" ht="19.5" spans="1:7">
+      <c r="A1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="40" t="s">
+    <row r="2" ht="15.75" spans="1:7">
+      <c r="A2" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="43" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="5"/>
@@ -3142,19 +3158,19 @@
       <c r="G3" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="30">
+      <c r="A6" s="31">
         <v>0</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="31">
         <v>1</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="31">
         <v>2</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="31">
         <v>3</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="31">
         <v>4</v>
       </c>
       <c r="F6">
@@ -3179,63 +3195,63 @@
       <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="12.9047619047619" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="12.9090909090909" style="30" customWidth="1"/>
-    <col min="6" max="6" width="30.9090909090909" customWidth="1"/>
-    <col min="7" max="7" width="22.2727272727273" customWidth="1"/>
-    <col min="8" max="16379" width="12.9090909090909" customWidth="1"/>
+    <col min="1" max="1" width="21.7238095238095" customWidth="1"/>
+    <col min="2" max="2" width="32.3619047619048" customWidth="1"/>
+    <col min="3" max="5" width="12.9047619047619" style="31" customWidth="1"/>
+    <col min="6" max="6" width="30.9047619047619" customWidth="1"/>
+    <col min="7" max="7" width="22.2761904761905" customWidth="1"/>
+    <col min="8" max="16379" width="12.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="34" t="s">
+    <row r="2" ht="15.75" spans="1:7">
+      <c r="A2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="35" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="30"/>
-      <c r="F3" s="36" t="s">
+      <c r="B3" s="31"/>
+      <c r="F3" s="37" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="5"/>
@@ -3247,13 +3263,13 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="31">
         <v>2</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="31">
         <v>3</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="31">
         <v>4</v>
       </c>
       <c r="F10">
@@ -3278,13 +3294,13 @@
       <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.9090909090909" customWidth="1"/>
+    <col min="1" max="1" width="22.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3303,17 +3319,17 @@
       <selection activeCell="A2" sqref="A2:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="18.0909090909091" customWidth="1"/>
-    <col min="2" max="2" width="22.4545454545455" customWidth="1"/>
+    <col min="1" max="1" width="18.0952380952381" customWidth="1"/>
+    <col min="2" max="2" width="22.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3329,41 +3345,41 @@
   <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.9047619047619" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
-    <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
-    <col min="7" max="7" width="27.6363636363636" style="16" customWidth="1"/>
-    <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
-    <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
-    <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
-    <col min="24" max="24" width="19.7272727272727" customWidth="1"/>
-    <col min="25" max="25" width="21.6363636363636" customWidth="1"/>
-    <col min="26" max="26" width="18.9090909090909" customWidth="1"/>
-    <col min="27" max="27" width="20.5454545454545" customWidth="1"/>
-    <col min="28" max="16384" width="10.9090909090909" customWidth="1"/>
+    <col min="1" max="5" width="21.3619047619048" customWidth="1"/>
+    <col min="6" max="6" width="11.4571428571429" customWidth="1"/>
+    <col min="7" max="7" width="27.6380952380952" style="17" customWidth="1"/>
+    <col min="8" max="8" width="9.36190476190476" customWidth="1"/>
+    <col min="9" max="22" width="21.3619047619048" customWidth="1"/>
+    <col min="23" max="23" width="16.4571428571429" customWidth="1"/>
+    <col min="24" max="24" width="19.7238095238095" customWidth="1"/>
+    <col min="25" max="25" width="21.6380952380952" customWidth="1"/>
+    <col min="26" max="26" width="18.9047619047619" customWidth="1"/>
+    <col min="27" max="27" width="20.5428571428571" customWidth="1"/>
+    <col min="28" max="16384" width="10.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="16" customFormat="1" ht="17" spans="1:27">
-      <c r="A1" s="17" t="s">
+    <row r="1" s="17" customFormat="1" ht="18" spans="1:27">
+      <c r="A1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>54</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3378,22 +3394,22 @@
       <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -3414,30 +3430,30 @@
       <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3446,13 +3462,13 @@
       <c r="E2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>83</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -3461,13 +3477,13 @@
       <c r="J2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="27" t="s">
         <v>88</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -3482,7 +3498,7 @@
       <c r="Q2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="21" t="s">
         <v>93</v>
       </c>
       <c r="S2" s="5" t="s">
@@ -3491,20 +3507,20 @@
       <c r="T2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="55" t="s">
+      <c r="U2" s="56" t="s">
         <v>96</v>
       </c>
       <c r="V2" s="5"/>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="56" t="s">
+      <c r="Y2" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="Z2" s="56" t="s">
+      <c r="Z2" s="57" t="s">
         <v>100</v>
       </c>
       <c r="AA2" s="5" t="s">
@@ -3515,13 +3531,13 @@
       <c r="E3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="26" t="s">
         <v>105</v>
       </c>
       <c r="U3" s="5" t="s">
@@ -3532,16 +3548,16 @@
       <c r="E4" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="24"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="24"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -3562,7 +3578,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="25">
         <v>6</v>
       </c>
       <c r="H8">
@@ -3627,130 +3643,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="24"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="24"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="24"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="24"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="24"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="24"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="24"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="24"/>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="24"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="24"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="24"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="24"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="24"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="24"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="24"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="24"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="24"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="24"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="24"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="24"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="24"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="24"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="24"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="24"/>
+      <c r="G35" s="25"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="24"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="24"/>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="24"/>
+      <c r="G38" s="25"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="24"/>
+      <c r="G39" s="25"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="24"/>
+      <c r="G40" s="25"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="24"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="24"/>
+      <c r="G42" s="25"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="24"/>
+      <c r="G43" s="25"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="24"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="24"/>
+      <c r="G45" s="25"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="24"/>
+      <c r="G46" s="25"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="24"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="24"/>
+      <c r="G48" s="25"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="24"/>
+      <c r="G49" s="25"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="24"/>
+      <c r="G50" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3767,21 +3783,21 @@
       <selection activeCell="C17" sqref="A2:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="19.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="20.6363636363636" customWidth="1"/>
-    <col min="3" max="3" width="11.1818181818182" customWidth="1"/>
+    <col min="1" max="1" width="19.2761904761905" customWidth="1"/>
+    <col min="2" max="2" width="20.6380952380952" customWidth="1"/>
+    <col min="3" max="3" width="11.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Login Feature and POM Updated
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="9" activeTab="13"/>
+    <workbookView windowWidth="18350" windowHeight="6950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="196">
   <si>
     <t>Environment Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>QA</t>
   </si>
   <si>
-    <t>https://gha.qa.xealei.com/</t>
+    <t>https://xat.qa.xealei.com/</t>
   </si>
   <si>
     <t>PRE-PROD</t>
@@ -65,22 +65,55 @@
     <t>assets/img/xealei-logo2.png</t>
   </si>
   <si>
-    <t>https://gha.qa.xealei.com/login</t>
+    <t>https://xat.qa.xealei.com/login</t>
   </si>
   <si>
     <t>Names</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>Email / Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
+    <t>FACILITY ADMIN</t>
+  </si>
+  <si>
     <t>mohamedra</t>
   </si>
   <si>
-    <t>xealei@23</t>
+    <t>auto@123</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>AStaff</t>
+  </si>
+  <si>
+    <t>CHIEF NURSE</t>
+  </si>
+  <si>
+    <t>AChief_Nu</t>
+  </si>
+  <si>
+    <t>RESIDENT MANAGER</t>
+  </si>
+  <si>
+    <t>AManager</t>
+  </si>
+  <si>
+    <t>CLINICAL COORDINATOR</t>
+  </si>
+  <si>
+    <t>AClinical</t>
+  </si>
+  <si>
+    <t>SOCIAL WORKER</t>
+  </si>
+  <si>
+    <t>ASWorker</t>
   </si>
   <si>
     <t>ALPHIND</t>
@@ -807,7 +840,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,13 +965,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1321,7 +1347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1368,19 +1394,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1499,133 +1512,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1704,16 +1717,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2062,7 +2075,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -2107,7 +2120,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://preprod.xealei.com/" tooltip="https://preprod.xealei.com/"/>
     <hyperlink ref="B4" r:id="rId2" display="https://www.xealei.com/"/>
-    <hyperlink ref="B2" r:id="rId3" display="https://gha.qa.xealei.com/"/>
+    <hyperlink ref="B2" r:id="rId3" display="https://xat.qa.xealei.com/" tooltip="https://xat.qa.xealei.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2119,7 +2132,7 @@
   <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
@@ -2140,188 +2153,188 @@
   <sheetData>
     <row r="1" s="16" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="17" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" ht="17.5" spans="1:27">
       <c r="A2" s="19" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F2" s="54" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="H2" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>105</v>
-      </c>
       <c r="M2" s="26" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="R2" s="28" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="S2" s="28" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="U2" s="55" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="V2" s="5"/>
       <c r="W2" s="56" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="X2" s="56" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="Y2" s="56" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="Z2" s="56" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="5" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="5" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="G4" s="24"/>
     </row>
@@ -2566,10 +2579,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2602,54 +2615,54 @@
   <sheetData>
     <row r="1" s="7" customFormat="1" spans="1:8">
       <c r="A1" s="8" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
       <c r="A2" s="56" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="H2" s="58" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2680,18 +2693,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="12" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="12" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2724,60 +2737,60 @@
   <sheetData>
     <row r="1" s="7" customFormat="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="H2" s="59" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="9:9">
@@ -2811,18 +2824,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="12" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="12" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2836,8 +2849,8 @@
   <sheetPr/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -2856,58 +2869,58 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17" spans="1:18">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" ht="87" spans="1:18">
@@ -2916,18 +2929,18 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -2955,7 +2968,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -2987,7 +3000,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://gha.qa.xealei.com/login"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://xat.qa.xealei.com/login" tooltip="https://xat.qa.xealei.com/login"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2997,15 +3010,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="22.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="16382" width="18" customWidth="1"/>
   </cols>
@@ -3023,52 +3036,111 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="44" t="s">
         <v>17</v>
       </c>
+      <c r="C2" s="45" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>20</v>
+      <c r="C4" s="45" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>20</v>
+      <c r="C5" s="45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mohamedra" tooltip="mailto:fa@xealei.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="xealei@23"/>
+    <hyperlink ref="C3" r:id="rId1" display="auto@123"/>
+    <hyperlink ref="C4" r:id="rId1" display="auto@123"/>
+    <hyperlink ref="C5" r:id="rId1" display="auto@123"/>
+    <hyperlink ref="C6" r:id="rId1" display="auto@123"/>
+    <hyperlink ref="C2" r:id="rId1" display="auto@123"/>
+    <hyperlink ref="C7" r:id="rId1" display="auto@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3096,45 +3168,45 @@
   <sheetData>
     <row r="1" s="37" customFormat="1" ht="19.5" spans="1:7">
       <c r="A1" s="31" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="40" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -3191,52 +3263,52 @@
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
       <c r="A1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>27</v>
-      </c>
       <c r="D1" s="31" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="34" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="30"/>
       <c r="F3" s="36" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -3285,7 +3357,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3311,10 +3383,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="29" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3349,188 +3421,188 @@
   <sheetData>
     <row r="1" s="16" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="17" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="19" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="F2" s="54" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="U2" s="55" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="V2" s="5"/>
       <c r="W2" s="56" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="X2" s="56" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="Y2" s="56" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="Z2" s="56" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="5" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="5" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G4" s="24"/>
     </row>
@@ -3776,13 +3848,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="9" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for IR Staff.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7200" firstSheet="9" activeTab="13"/>
+    <workbookView windowWidth="19635" windowHeight="7650" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
   <si>
     <t>Environment Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>QA</t>
   </si>
   <si>
-    <t>https://gha.qa.xealei.com/</t>
+    <t>https://xat.qa.xealei.com/</t>
   </si>
   <si>
     <t>PRE-PROD</t>
@@ -785,6 +785,18 @@
     <t>Notification Method</t>
   </si>
   <si>
+    <t>Created Inj.Description</t>
+  </si>
+  <si>
+    <t>Albert Nicholas</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -794,7 +806,25 @@
     <t>Head , Face , Left Shoulder , Right Shoulder , Left Arm , Right Arm ,  Back , Hip , Left Wrist , Right Wrist , Left Knee , Right Knee , Left Foot , Right Foot</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
     <t>Abrasion , Bleeding , Bruise , Scratch</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Phone Call</t>
   </si>
 </sst>
 </file>
@@ -1630,19 +1660,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2066,7 +2099,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -2076,34 +2109,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="54" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="55" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2111,7 +2144,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://preprod.xealei.com/" tooltip="https://preprod.xealei.com/"/>
     <hyperlink ref="B4" r:id="rId2" display="https://www.xealei.com/"/>
-    <hyperlink ref="B2" r:id="rId3" display="https://gha.qa.xealei.com/"/>
+    <hyperlink ref="B2" r:id="rId3" display="https://xat.qa.xealei.com/" tooltip="https://xat.qa.xealei.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2131,7 +2164,7 @@
   <cols>
     <col min="1" max="5" width="21.3619047619048" customWidth="1"/>
     <col min="6" max="6" width="11.4571428571429" customWidth="1"/>
-    <col min="7" max="7" width="27.6380952380952" style="17" customWidth="1"/>
+    <col min="7" max="7" width="27.6380952380952" style="20" customWidth="1"/>
     <col min="8" max="8" width="9.36190476190476" customWidth="1"/>
     <col min="9" max="22" width="21.3619047619048" customWidth="1"/>
     <col min="23" max="23" width="16.4571428571429" customWidth="1"/>
@@ -2142,23 +2175,23 @@
     <col min="28" max="16383" width="10.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="1" ht="18" spans="1:27">
-      <c r="A1" s="18" t="s">
+    <row r="1" s="20" customFormat="1" ht="18" spans="1:27">
+      <c r="A1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="22" t="s">
         <v>54</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2173,22 +2206,22 @@
       <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="22" t="s">
         <v>64</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -2209,30 +2242,30 @@
       <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" ht="17.25" spans="1:27">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>111</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2241,13 +2274,13 @@
       <c r="E2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="27" t="s">
         <v>115</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -2256,13 +2289,13 @@
       <c r="J2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="30" t="s">
         <v>118</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -2277,29 +2310,29 @@
       <c r="Q2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="R2" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="32" t="s">
         <v>124</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="56" t="s">
+      <c r="U2" s="59" t="s">
         <v>96</v>
       </c>
       <c r="V2" s="5"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="57" t="s">
+      <c r="X2" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="57" t="s">
+      <c r="Y2" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="Z2" s="57" t="s">
+      <c r="Z2" s="60" t="s">
         <v>100</v>
       </c>
       <c r="AA2" s="5" t="s">
@@ -2310,13 +2343,13 @@
       <c r="E3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="31" t="s">
         <v>87</v>
       </c>
       <c r="U3" s="5" t="s">
@@ -2327,16 +2360,16 @@
       <c r="E4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="25"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="25"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="25"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -2357,7 +2390,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="28">
         <v>6</v>
       </c>
       <c r="H8">
@@ -2422,130 +2455,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="25"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="25"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="25"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="25"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="25"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="25"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="25"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="25"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="25"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="25"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="25"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="25"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="25"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="25"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="25"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="25"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="25"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="25"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="25"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="25"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="25"/>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="25"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="25"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="25"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="25"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="25"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="25"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="25"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="25"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="25"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="25"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="25"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="25"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="25"/>
+      <c r="G42" s="28"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="25"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="25"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="25"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="25"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="25"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="25"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="25"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="25"/>
+      <c r="G50" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2569,10 +2602,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2604,55 +2637,55 @@
     <col min="9" max="16384" width="19.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" spans="1:8">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="11" customFormat="1" spans="1:8">
+      <c r="A1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="13" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:8">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="60" t="s">
         <v>141</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="62" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2683,18 +2716,18 @@
       </c>
     </row>
     <row r="6" ht="17.25" spans="7:8">
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="17" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="7" ht="17.25" spans="7:8">
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="17" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2726,32 +2759,32 @@
     <col min="9" max="16384" width="19.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="11" customFormat="1" spans="1:9">
+      <c r="A1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="18" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2762,22 +2795,22 @@
       <c r="B2" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="63" t="s">
         <v>161</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -2814,18 +2847,18 @@
       </c>
     </row>
     <row r="6" ht="17.25" spans="7:8">
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="17" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="7" ht="17.25" spans="7:8">
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="17" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2838,10 +2871,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0952380952381" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2855,10 +2888,12 @@
     <col min="8" max="9" width="20.0952380952381" customWidth="1"/>
     <col min="10" max="10" width="30.6380952380952" customWidth="1"/>
     <col min="11" max="11" width="18.5428571428571" customWidth="1"/>
-    <col min="12" max="16384" width="20.0952380952381" customWidth="1"/>
+    <col min="12" max="18" width="20.0952380952381" customWidth="1"/>
+    <col min="19" max="19" width="26.4285714285714" customWidth="1"/>
+    <col min="20" max="16384" width="20.0952380952381" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="18" spans="1:18">
+    <row r="1" s="1" customFormat="1" ht="18" spans="1:19">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
@@ -2913,34 +2948,66 @@
       <c r="R1" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="2" ht="90" spans="1:18">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="S1" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" ht="90" spans="1:19">
+      <c r="A2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44938</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="E2" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
+        <v>185</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="O2" s="6">
+        <v>44938</v>
+      </c>
+      <c r="P2" s="5">
+        <v>1134</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S2" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2982,21 +3049,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="52" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="5"/>
@@ -3027,57 +3094,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="47" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="50" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="40" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="40" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3102,54 +3169,54 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.6380952380952" style="31" customWidth="1"/>
-    <col min="2" max="2" width="28.7238095238095" style="31" customWidth="1"/>
-    <col min="3" max="5" width="12.6380952380952" style="31" customWidth="1"/>
+    <col min="1" max="1" width="12.6380952380952" style="34" customWidth="1"/>
+    <col min="2" max="2" width="28.7238095238095" style="34" customWidth="1"/>
+    <col min="3" max="5" width="12.6380952380952" style="34" customWidth="1"/>
     <col min="6" max="6" width="20.2761904761905" customWidth="1"/>
     <col min="7" max="7" width="16.8190476190476" customWidth="1"/>
     <col min="8" max="16381" width="12.6380952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="1" ht="19.5" spans="1:7">
-      <c r="A1" s="32" t="s">
+    <row r="1" s="41" customFormat="1" ht="19.5" spans="1:7">
+      <c r="A1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:7">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="46" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="5"/>
@@ -3158,19 +3225,19 @@
       <c r="G3" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="31">
+      <c r="A6" s="34">
         <v>0</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="34">
         <v>1</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="34">
         <v>2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="34">
         <v>3</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="34">
         <v>4</v>
       </c>
       <c r="F6">
@@ -3199,59 +3266,59 @@
   <cols>
     <col min="1" max="1" width="21.7238095238095" customWidth="1"/>
     <col min="2" max="2" width="32.3619047619048" customWidth="1"/>
-    <col min="3" max="5" width="12.9047619047619" style="31" customWidth="1"/>
+    <col min="3" max="5" width="12.9047619047619" style="34" customWidth="1"/>
     <col min="6" max="6" width="30.9047619047619" customWidth="1"/>
     <col min="7" max="7" width="22.2761904761905" customWidth="1"/>
     <col min="8" max="16379" width="12.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:7">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="38" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="B3" s="34"/>
+      <c r="F3" s="40" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="5"/>
@@ -3263,13 +3330,13 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="34">
         <v>2</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="34">
         <v>3</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="34">
         <v>4</v>
       </c>
       <c r="F10">
@@ -3300,7 +3367,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3326,10 +3393,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3352,7 +3419,7 @@
   <cols>
     <col min="1" max="5" width="21.3619047619048" customWidth="1"/>
     <col min="6" max="6" width="11.4571428571429" customWidth="1"/>
-    <col min="7" max="7" width="27.6380952380952" style="17" customWidth="1"/>
+    <col min="7" max="7" width="27.6380952380952" style="20" customWidth="1"/>
     <col min="8" max="8" width="9.36190476190476" customWidth="1"/>
     <col min="9" max="22" width="21.3619047619048" customWidth="1"/>
     <col min="23" max="23" width="16.4571428571429" customWidth="1"/>
@@ -3363,23 +3430,23 @@
     <col min="28" max="16384" width="10.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="1" ht="18" spans="1:27">
-      <c r="A1" s="18" t="s">
+    <row r="1" s="20" customFormat="1" ht="18" spans="1:27">
+      <c r="A1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="22" t="s">
         <v>54</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3394,22 +3461,22 @@
       <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="22" t="s">
         <v>64</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -3430,30 +3497,30 @@
       <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3462,13 +3529,13 @@
       <c r="E2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -3477,13 +3544,13 @@
       <c r="J2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="30" t="s">
         <v>88</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -3498,7 +3565,7 @@
       <c r="Q2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="24" t="s">
         <v>93</v>
       </c>
       <c r="S2" s="5" t="s">
@@ -3507,20 +3574,20 @@
       <c r="T2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="56" t="s">
+      <c r="U2" s="59" t="s">
         <v>96</v>
       </c>
       <c r="V2" s="5"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="57" t="s">
+      <c r="X2" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="57" t="s">
+      <c r="Y2" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="Z2" s="57" t="s">
+      <c r="Z2" s="60" t="s">
         <v>100</v>
       </c>
       <c r="AA2" s="5" t="s">
@@ -3531,13 +3598,13 @@
       <c r="E3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="29" t="s">
         <v>105</v>
       </c>
       <c r="U3" s="5" t="s">
@@ -3548,16 +3615,16 @@
       <c r="E4" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="25"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="25"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="25"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -3578,7 +3645,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="28">
         <v>6</v>
       </c>
       <c r="H8">
@@ -3643,130 +3710,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="25"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="25"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="25"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="25"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="25"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="25"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="25"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="25"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="25"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="25"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="25"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="25"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="25"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="25"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="25"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="25"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="25"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="25"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="25"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="25"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="25"/>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="25"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="25"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="25"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="25"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="25"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="25"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="25"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="25"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="25"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="25"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="25"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="25"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="25"/>
+      <c r="G42" s="28"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="25"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="25"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="25"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="25"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="25"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="25"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="25"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="25"/>
+      <c r="G50" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3791,13 +3858,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IR flow for staff latest changes.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="194">
   <si>
     <t>Environment Name</t>
   </si>
@@ -822,9 +822,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>Phone Call</t>
   </si>
 </sst>
 </file>
@@ -2871,8 +2868,8 @@
   <sheetPr/>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0952380952381" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3003,7 +3000,7 @@
         <v>193</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>194</v>
+        <v>14</v>
       </c>
       <c r="S2" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added ToolTip text code.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="225">
   <si>
     <t>Environment Name</t>
   </si>
@@ -788,6 +788,18 @@
     <t>Created Inj.Description</t>
   </si>
   <si>
+    <t>Created Report ID</t>
+  </si>
+  <si>
+    <t>Cheif Nurse reviewer approved comments</t>
+  </si>
+  <si>
+    <t>Residential Manager reviewer approved comments</t>
+  </si>
+  <si>
+    <t>Social Worker reviewer approved comments</t>
+  </si>
+  <si>
     <t>Arlia Thomas</t>
   </si>
   <si>
@@ -822,6 +834,87 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>test - -51:44</t>
+  </si>
+  <si>
+    <t>IR00029</t>
+  </si>
+  <si>
+    <t>cheif nurse approved.</t>
+  </si>
+  <si>
+    <t>Residential Manager approved.</t>
+  </si>
+  <si>
+    <t>Social Worker approved.</t>
+  </si>
+  <si>
+    <t>Cheif nurse rejected.</t>
+  </si>
+  <si>
+    <t>Residential Manager rejected.</t>
+  </si>
+  <si>
+    <t>Social Worker rejected.</t>
+  </si>
+  <si>
+    <t>test - -57:40</t>
+  </si>
+  <si>
+    <t>IR00032</t>
+  </si>
+  <si>
+    <t>test - -00:23</t>
+  </si>
+  <si>
+    <t>test - -01:57</t>
+  </si>
+  <si>
+    <t>IR00033</t>
+  </si>
+  <si>
+    <t>test - -16:21</t>
+  </si>
+  <si>
+    <t>IR00034</t>
+  </si>
+  <si>
+    <t>test - -17:55</t>
+  </si>
+  <si>
+    <t>IR00035</t>
+  </si>
+  <si>
+    <t>test - -20:08</t>
+  </si>
+  <si>
+    <t>IR00036</t>
+  </si>
+  <si>
+    <t>test - -22:23</t>
+  </si>
+  <si>
+    <t>IR00037</t>
+  </si>
+  <si>
+    <t>test - -26:48</t>
+  </si>
+  <si>
+    <t>IR00038</t>
+  </si>
+  <si>
+    <t>test - -28:04</t>
+  </si>
+  <si>
+    <t>IR00039</t>
+  </si>
+  <si>
+    <t>test - -44:32</t>
+  </si>
+  <si>
+    <t>IR00040</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1750,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2099,8 +2192,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.3619047619048" customWidth="1"/>
-    <col min="2" max="2" width="29.0952380952381" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.3619047619048"/>
+    <col min="2" max="2" customWidth="true" width="29.0952380952381"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2157,17 +2250,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9047619047619" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="21.3619047619048" customWidth="1"/>
-    <col min="6" max="6" width="11.4571428571429" customWidth="1"/>
-    <col min="7" max="7" width="27.6380952380952" style="18" customWidth="1"/>
-    <col min="8" max="8" width="9.36190476190476" customWidth="1"/>
-    <col min="9" max="22" width="21.3619047619048" customWidth="1"/>
-    <col min="23" max="23" width="16.4571428571429" customWidth="1"/>
-    <col min="24" max="24" width="19.7238095238095" customWidth="1"/>
-    <col min="25" max="25" width="21.6380952380952" customWidth="1"/>
-    <col min="26" max="26" width="18.9047619047619" customWidth="1"/>
-    <col min="27" max="27" width="20.5428571428571" customWidth="1"/>
-    <col min="28" max="16383" width="10.9047619047619" customWidth="1"/>
+    <col min="1" max="5" customWidth="true" width="21.3619047619048"/>
+    <col min="6" max="6" customWidth="true" width="11.4571428571429"/>
+    <col min="7" max="7" customWidth="true" style="18" width="27.6380952380952"/>
+    <col min="8" max="8" customWidth="true" width="9.36190476190476"/>
+    <col min="9" max="22" customWidth="true" width="21.3619047619048"/>
+    <col min="23" max="23" customWidth="true" width="16.4571428571429"/>
+    <col min="24" max="24" customWidth="true" width="19.7238095238095"/>
+    <col min="25" max="25" customWidth="true" width="21.6380952380952"/>
+    <col min="26" max="26" customWidth="true" width="18.9047619047619"/>
+    <col min="27" max="27" customWidth="true" width="20.5428571428571"/>
+    <col min="28" max="16383" customWidth="true" width="10.9047619047619"/>
   </cols>
   <sheetData>
     <row r="1" s="18" customFormat="1" ht="18" spans="1:27">
@@ -2592,8 +2685,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="23.6380952380952" customWidth="1"/>
-    <col min="2" max="2" width="29.2761904761905" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.6380952380952"/>
+    <col min="2" max="2" customWidth="true" width="29.2761904761905"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2621,15 +2714,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1809523809524" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.2761904761905" customWidth="1"/>
-    <col min="2" max="2" width="23.2761904761905" customWidth="1"/>
-    <col min="3" max="3" width="21.3619047619048" customWidth="1"/>
-    <col min="4" max="4" width="19.1809523809524" customWidth="1"/>
-    <col min="5" max="5" width="12.6380952380952" customWidth="1"/>
-    <col min="6" max="6" width="12.0952380952381" customWidth="1"/>
-    <col min="7" max="7" width="12.1809523809524" customWidth="1"/>
-    <col min="8" max="8" width="46.0952380952381" customWidth="1"/>
-    <col min="9" max="16384" width="19.1809523809524" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.2761904761905"/>
+    <col min="2" max="2" customWidth="true" width="23.2761904761905"/>
+    <col min="3" max="3" customWidth="true" width="21.3619047619048"/>
+    <col min="4" max="4" customWidth="true" width="19.1809523809524"/>
+    <col min="5" max="5" customWidth="true" width="12.6380952380952"/>
+    <col min="6" max="6" customWidth="true" width="12.0952380952381"/>
+    <col min="7" max="7" customWidth="true" width="12.1809523809524"/>
+    <col min="8" max="8" customWidth="true" width="46.0952380952381"/>
+    <col min="9" max="16384" customWidth="true" width="19.1809523809524"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="1" spans="1:8">
@@ -2743,15 +2836,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1809523809524" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="13.2761904761905" customWidth="1"/>
-    <col min="2" max="2" width="23.2761904761905" customWidth="1"/>
-    <col min="3" max="3" width="21.3619047619048" customWidth="1"/>
-    <col min="4" max="4" width="19.1809523809524" customWidth="1"/>
-    <col min="5" max="5" width="12.6380952380952" customWidth="1"/>
-    <col min="6" max="6" width="12.0952380952381" customWidth="1"/>
-    <col min="7" max="7" width="12.1809523809524" customWidth="1"/>
-    <col min="8" max="8" width="46.0952380952381" customWidth="1"/>
-    <col min="9" max="16384" width="19.1809523809524" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.2761904761905"/>
+    <col min="2" max="2" customWidth="true" width="23.2761904761905"/>
+    <col min="3" max="3" customWidth="true" width="21.3619047619048"/>
+    <col min="4" max="4" customWidth="true" width="19.1809523809524"/>
+    <col min="5" max="5" customWidth="true" width="12.6380952380952"/>
+    <col min="6" max="6" customWidth="true" width="12.0952380952381"/>
+    <col min="7" max="7" customWidth="true" width="12.1809523809524"/>
+    <col min="8" max="8" customWidth="true" width="46.0952380952381"/>
+    <col min="9" max="16384" customWidth="true" width="19.1809523809524"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="1" spans="1:9">
@@ -2866,29 +2959,36 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0952380952381" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="2" width="20.0952380952381" customWidth="1"/>
-    <col min="3" max="3" width="24.2761904761905" customWidth="1"/>
-    <col min="4" max="4" width="20.0952380952381" customWidth="1"/>
-    <col min="5" max="5" width="24.2761904761905" customWidth="1"/>
-    <col min="6" max="6" width="25.5428571428571" customWidth="1"/>
-    <col min="7" max="7" width="25.2761904761905" customWidth="1"/>
-    <col min="8" max="9" width="20.0952380952381" customWidth="1"/>
-    <col min="10" max="10" width="30.6380952380952" customWidth="1"/>
-    <col min="11" max="11" width="18.5428571428571" customWidth="1"/>
-    <col min="12" max="18" width="20.0952380952381" customWidth="1"/>
-    <col min="19" max="19" width="26.4285714285714" customWidth="1"/>
-    <col min="20" max="16384" width="20.0952380952381" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="20.0952380952381"/>
+    <col min="3" max="3" customWidth="true" width="24.2761904761905"/>
+    <col min="4" max="4" customWidth="true" width="20.0952380952381"/>
+    <col min="5" max="5" customWidth="true" width="24.2761904761905"/>
+    <col min="6" max="6" customWidth="true" width="25.5428571428571"/>
+    <col min="7" max="7" customWidth="true" width="25.2761904761905"/>
+    <col min="8" max="9" customWidth="true" width="20.0952380952381"/>
+    <col min="10" max="10" customWidth="true" width="30.6380952380952"/>
+    <col min="11" max="11" customWidth="true" width="18.5428571428571"/>
+    <col min="12" max="18" customWidth="true" width="20.0952380952381"/>
+    <col min="19" max="19" customWidth="true" width="26.4285714285714"/>
+    <col min="20" max="20" customWidth="true" width="22.1428571428571"/>
+    <col min="21" max="21" customWidth="true" width="47.1428571428571"/>
+    <col min="22" max="22" customWidth="true" width="54.7142857142857"/>
+    <col min="23" max="23" customWidth="true" width="47.1428571428571"/>
+    <col min="24" max="24" customWidth="true" width="44.8571428571429"/>
+    <col min="25" max="25" customWidth="true" width="55.0"/>
+    <col min="26" max="26" customWidth="true" width="46.7142857142857"/>
+    <col min="27" max="16384" customWidth="true" width="20.0952380952381"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="18" spans="1:19">
+    <row r="1" s="1" customFormat="1" ht="18" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
@@ -2946,46 +3046,67 @@
       <c r="S1" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="2" ht="90" spans="1:19">
+      <c r="T1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" ht="90" spans="1:26">
       <c r="A2" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" s="6">
         <v>44938</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>95</v>
@@ -2997,12 +3118,35 @@
         <v>1134</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="5"/>
+      <c r="S2" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -3038,9 +3182,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="31.2761904761905" customWidth="1"/>
-    <col min="2" max="2" width="27.3619047619048" customWidth="1"/>
-    <col min="3" max="3" width="14.2761904761905" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.2761904761905"/>
+    <col min="2" max="2" customWidth="true" width="27.3619047619048"/>
+    <col min="3" max="3" customWidth="true" width="14.2761904761905"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3083,9 +3227,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="16382" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0"/>
+    <col min="2" max="2" customWidth="true" width="34.0"/>
+    <col min="3" max="16382" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3164,12 +3308,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.6380952380952" style="32" customWidth="1"/>
-    <col min="2" max="2" width="28.7238095238095" style="32" customWidth="1"/>
-    <col min="3" max="5" width="12.6380952380952" style="32" customWidth="1"/>
-    <col min="6" max="6" width="20.2761904761905" customWidth="1"/>
-    <col min="7" max="7" width="16.8190476190476" customWidth="1"/>
-    <col min="8" max="16381" width="12.6380952380952" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="32" width="12.6380952380952"/>
+    <col min="2" max="2" customWidth="true" style="32" width="28.7238095238095"/>
+    <col min="3" max="5" customWidth="true" style="32" width="12.6380952380952"/>
+    <col min="6" max="6" customWidth="true" width="20.2761904761905"/>
+    <col min="7" max="7" customWidth="true" width="16.8190476190476"/>
+    <col min="8" max="16381" customWidth="true" width="12.6380952380952"/>
   </cols>
   <sheetData>
     <row r="1" s="39" customFormat="1" ht="19.5" spans="1:7">
@@ -3259,12 +3403,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9047619047619" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.7238095238095" customWidth="1"/>
-    <col min="2" max="2" width="32.3619047619048" customWidth="1"/>
-    <col min="3" max="5" width="12.9047619047619" style="32" customWidth="1"/>
-    <col min="6" max="6" width="30.9047619047619" customWidth="1"/>
-    <col min="7" max="7" width="22.2761904761905" customWidth="1"/>
-    <col min="8" max="16379" width="12.9047619047619" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7238095238095"/>
+    <col min="2" max="2" customWidth="true" width="32.3619047619048"/>
+    <col min="3" max="5" customWidth="true" style="32" width="12.9047619047619"/>
+    <col min="6" max="6" customWidth="true" width="30.9047619047619"/>
+    <col min="7" max="7" customWidth="true" width="22.2761904761905"/>
+    <col min="8" max="16379" customWidth="true" width="12.9047619047619"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
@@ -3358,7 +3502,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.9047619047619" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.9047619047619"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -3383,8 +3527,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="18.0952380952381" customWidth="1"/>
-    <col min="2" max="2" width="22.4571428571429" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0952380952381"/>
+    <col min="2" max="2" customWidth="true" width="22.4571428571429"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3412,17 +3556,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9047619047619" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="21.3619047619048" customWidth="1"/>
-    <col min="6" max="6" width="11.4571428571429" customWidth="1"/>
-    <col min="7" max="7" width="27.6380952380952" style="18" customWidth="1"/>
-    <col min="8" max="8" width="9.36190476190476" customWidth="1"/>
-    <col min="9" max="22" width="21.3619047619048" customWidth="1"/>
-    <col min="23" max="23" width="16.4571428571429" customWidth="1"/>
-    <col min="24" max="24" width="19.7238095238095" customWidth="1"/>
-    <col min="25" max="25" width="21.6380952380952" customWidth="1"/>
-    <col min="26" max="26" width="18.9047619047619" customWidth="1"/>
-    <col min="27" max="27" width="20.5428571428571" customWidth="1"/>
-    <col min="28" max="16384" width="10.9047619047619" customWidth="1"/>
+    <col min="1" max="5" customWidth="true" width="21.3619047619048"/>
+    <col min="6" max="6" customWidth="true" width="11.4571428571429"/>
+    <col min="7" max="7" customWidth="true" style="18" width="27.6380952380952"/>
+    <col min="8" max="8" customWidth="true" width="9.36190476190476"/>
+    <col min="9" max="22" customWidth="true" width="21.3619047619048"/>
+    <col min="23" max="23" customWidth="true" width="16.4571428571429"/>
+    <col min="24" max="24" customWidth="true" width="19.7238095238095"/>
+    <col min="25" max="25" customWidth="true" width="21.6380952380952"/>
+    <col min="26" max="26" customWidth="true" width="18.9047619047619"/>
+    <col min="27" max="27" customWidth="true" width="20.5428571428571"/>
+    <col min="28" max="16384" customWidth="true" width="10.9047619047619"/>
   </cols>
   <sheetData>
     <row r="1" s="18" customFormat="1" ht="18" spans="1:27">
@@ -3847,9 +3991,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="19.2761904761905" customWidth="1"/>
-    <col min="2" max="2" width="20.6380952380952" customWidth="1"/>
-    <col min="3" max="3" width="11.1809523809524" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.2761904761905"/>
+    <col min="2" max="2" customWidth="true" width="20.6380952380952"/>
+    <col min="3" max="3" customWidth="true" width="11.1809523809524"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Added code for all approve till cheif nurse.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="249">
   <si>
     <t>Environment Name</t>
   </si>
@@ -915,6 +915,78 @@
   </si>
   <si>
     <t>IR00040</t>
+  </si>
+  <si>
+    <t>test - -55:34</t>
+  </si>
+  <si>
+    <t>IR00041</t>
+  </si>
+  <si>
+    <t>test - -58:04</t>
+  </si>
+  <si>
+    <t>IR00042</t>
+  </si>
+  <si>
+    <t>test - -03:17</t>
+  </si>
+  <si>
+    <t>IR00043</t>
+  </si>
+  <si>
+    <t>test - -10:12</t>
+  </si>
+  <si>
+    <t>IR00045</t>
+  </si>
+  <si>
+    <t>test - -12:48</t>
+  </si>
+  <si>
+    <t>IR00046</t>
+  </si>
+  <si>
+    <t>test - -18:45</t>
+  </si>
+  <si>
+    <t>IR00047</t>
+  </si>
+  <si>
+    <t>test - -22:05</t>
+  </si>
+  <si>
+    <t>IR00048</t>
+  </si>
+  <si>
+    <t>test - -28:11</t>
+  </si>
+  <si>
+    <t>IR00049</t>
+  </si>
+  <si>
+    <t>test - -04:03</t>
+  </si>
+  <si>
+    <t>IR00050</t>
+  </si>
+  <si>
+    <t>test - -10:37</t>
+  </si>
+  <si>
+    <t>IR00051</t>
+  </si>
+  <si>
+    <t>test - -36:24</t>
+  </si>
+  <si>
+    <t>IR00052</t>
+  </si>
+  <si>
+    <t>test - -40:59</t>
+  </si>
+  <si>
+    <t>IR00053</t>
   </si>
 </sst>
 </file>
@@ -3124,10 +3196,10 @@
         <v>14</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>200</v>

</xml_diff>

<commit_message>
Calender field scripts added
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7650" firstSheet="9" activeTab="13"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="290">
   <si>
     <t>Environment Name</t>
   </si>
@@ -75,15 +75,6 @@
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>mohamedra</t>
-  </si>
-  <si>
-    <t>xealei@23</t>
-  </si>
-  <si>
-    <t>ALPHIND</t>
   </si>
   <si>
     <r>
@@ -94,7 +85,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>alphindadmin@xealei.com</t>
+      <t>FACILITY ADMIN</t>
     </r>
   </si>
   <si>
@@ -106,11 +97,11 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>A!ph!nd@dm!n</t>
+      <t>mohamedra</t>
     </r>
   </si>
   <si>
-    <t>GHA</t>
+    <t>auto@123</t>
   </si>
   <si>
     <r>
@@ -121,11 +112,8 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ghaadmin@xealei.com</t>
+      <t>STAFF</t>
     </r>
-  </si>
-  <si>
-    <t>XEALEI</t>
   </si>
   <si>
     <r>
@@ -136,10 +124,106 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>xliadmin@xealei.com</t>
+      <t>AStaff</t>
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CHIEF NURSE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AChief_Nu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RESIDENT MANAGER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AManager</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CLINICAL COORDINATOR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AClinical</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOCIAL WORKER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASWorker</t>
+    </r>
+  </si>
+  <si>
     <t>SuiteName*</t>
   </si>
   <si>
@@ -179,6 +263,12 @@
     <t>Available</t>
   </si>
   <si>
+    <t>Suite-10:48:51</t>
+  </si>
+  <si>
+    <t>Suite-10:41:56</t>
+  </si>
+  <si>
     <t>Update SuiteName</t>
   </si>
   <si>
@@ -204,6 +294,9 @@
   </si>
   <si>
     <t>CreatedSuites</t>
+  </si>
+  <si>
+    <t>Suite-10:37:23</t>
   </si>
   <si>
     <t>Created SuiteName</t>
@@ -788,13 +881,19 @@
     <t>Created Inj.Description</t>
   </si>
   <si>
-    <t>Albert Nicholas</t>
+    <t>Selected Individual</t>
+  </si>
+  <si>
+    <t>Arlia Thomas</t>
+  </si>
+  <si>
+    <t>01/05/202406:47PM</t>
   </si>
   <si>
     <t>d</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Twisted Ankle</t>
   </si>
   <si>
     <t>Yes</t>
@@ -824,10 +923,265 @@
     <t>a</t>
   </si>
   <si>
-    <t>Phone Call</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-19:57</t>
+    <t>Twisted Ankle-40:36</t>
+  </si>
+  <si>
+    <t>01/08/202412:48PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-48:27</t>
+  </si>
+  <si>
+    <t>01/08/202412:53PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-53:39</t>
+  </si>
+  <si>
+    <t>01/08/202412:54PM</t>
+  </si>
+  <si>
+    <t>01/08/202412:58PM</t>
+  </si>
+  <si>
+    <t>01/08/202412:59PM</t>
+  </si>
+  <si>
+    <t>01/08/202401:19PM</t>
+  </si>
+  <si>
+    <t>01/08/202401:20PM</t>
+  </si>
+  <si>
+    <t>01/08/202401:24PM</t>
+  </si>
+  <si>
+    <t>01/08/202401:25PM</t>
+  </si>
+  <si>
+    <t>01/08/202401:40PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:11PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:15PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:32PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:33PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:38PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:40PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:41PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:45PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:48PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:51PM</t>
+  </si>
+  <si>
+    <t>01/08/202403:52PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:06PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:07PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:09PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:10PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:13PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:14PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:15PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:16PM</t>
+  </si>
+  <si>
+    <t>01/08/202404:17PM</t>
+  </si>
+  <si>
+    <t>01/08/202405:41PM</t>
+  </si>
+  <si>
+    <t>01/08/202405:46PM</t>
+  </si>
+  <si>
+    <t>01/08/202406:20PM</t>
+  </si>
+  <si>
+    <t>01/08/202406:31PM</t>
+  </si>
+  <si>
+    <t>01/09/202411:43AM</t>
+  </si>
+  <si>
+    <t>01/09/202411:45AM</t>
+  </si>
+  <si>
+    <t>01/09/202411:59AM</t>
+  </si>
+  <si>
+    <t>01/09/202412:02PM</t>
+  </si>
+  <si>
+    <t>01/10/202411:41AM</t>
+  </si>
+  <si>
+    <t>01/10/202411:46AM</t>
+  </si>
+  <si>
+    <t>01/10/202411:53AM</t>
+  </si>
+  <si>
+    <t>01/10/202412:03PM</t>
+  </si>
+  <si>
+    <t>01/10/202412:09PM</t>
+  </si>
+  <si>
+    <t>01/10/202412:12PM</t>
+  </si>
+  <si>
+    <t>01/10/202412:13PM</t>
+  </si>
+  <si>
+    <t>01/10/202412:22PM</t>
+  </si>
+  <si>
+    <t>01/10/202401:02PM</t>
+  </si>
+  <si>
+    <t>01/10/202401:04PM</t>
+  </si>
+  <si>
+    <t>01/10/202401:06PM</t>
+  </si>
+  <si>
+    <t>01/10/202401:09PM</t>
+  </si>
+  <si>
+    <t>01/10/202401:10PM</t>
+  </si>
+  <si>
+    <t>01/10/202401:12PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:00PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:02PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:04PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:08PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:15PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:23PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:25PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:28PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:31PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:33PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:34PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:40PM</t>
+  </si>
+  <si>
+    <t>01/10/202406:42PM</t>
+  </si>
+  <si>
+    <t>01/11/202411:37AM</t>
+  </si>
+  <si>
+    <t>01/11/202401:30PM</t>
+  </si>
+  <si>
+    <t>01/11/202401:34PM</t>
+  </si>
+  <si>
+    <t>01/11/202403:39PM</t>
+  </si>
+  <si>
+    <t>01/11/202404:31PM</t>
+  </si>
+  <si>
+    <t>01/11/202404:39PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-39:22</t>
+  </si>
+  <si>
+    <t>01/11/202404:47PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-47:53</t>
+  </si>
+  <si>
+    <t>01/11/202404:48PM</t>
+  </si>
+  <si>
+    <t>01/11/202404:54PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-54:44</t>
+  </si>
+  <si>
+    <t>01/11/202405:04PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-04:37</t>
+  </si>
+  <si>
+    <t>01/11/202406:00PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-00:07</t>
+  </si>
+  <si>
+    <t>01/11/202406:46PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-46:48</t>
+  </si>
+  <si>
+    <t>01/11/202406:47PM</t>
   </si>
 </sst>
 </file>
@@ -835,13 +1189,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,22 +1321,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -1355,7 +1702,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1402,19 +1749,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1521,164 +1855,162 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1701,7 +2033,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1744,24 +2076,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1770,7 +2093,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
@@ -2102,44 +2425,44 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.3619047619048"/>
-    <col min="2" max="2" customWidth="true" width="29.0952380952381"/>
+    <col min="1" max="1" customWidth="true" width="17.3636363636364"/>
+    <col min="2" max="2" customWidth="true" width="29.0909090909091"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="50" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="49" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="50" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2159,220 +2482,220 @@
   <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9047619047619" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" customWidth="true" width="21.3619047619048"/>
-    <col min="6" max="6" customWidth="true" width="11.4571428571429"/>
-    <col min="7" max="7" customWidth="true" style="20" width="27.6380952380952"/>
-    <col min="8" max="8" customWidth="true" width="9.36190476190476"/>
-    <col min="9" max="22" customWidth="true" width="21.3619047619048"/>
-    <col min="23" max="23" customWidth="true" width="16.4571428571429"/>
-    <col min="24" max="24" customWidth="true" width="19.7238095238095"/>
-    <col min="25" max="25" customWidth="true" width="21.6380952380952"/>
-    <col min="26" max="26" customWidth="true" width="18.9047619047619"/>
-    <col min="27" max="27" customWidth="true" width="20.5428571428571"/>
-    <col min="28" max="16383" customWidth="true" width="10.9047619047619"/>
+    <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
+    <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
+    <col min="7" max="7" customWidth="true" style="18" width="27.6363636363636"/>
+    <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
+    <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
+    <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
+    <col min="24" max="24" customWidth="true" width="19.7272727272727"/>
+    <col min="25" max="25" customWidth="true" width="21.6363636363636"/>
+    <col min="26" max="26" customWidth="true" width="18.9090909090909"/>
+    <col min="27" max="27" customWidth="true" width="20.5454545454545"/>
+    <col min="28" max="16383" customWidth="true" width="10.9090909090909"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="18" spans="1:27">
-      <c r="A1" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>54</v>
+    <row r="1" s="18" customFormat="1" ht="17" spans="1:27">
+      <c r="A1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" ht="17.25" spans="1:27">
-      <c r="A2" s="23" t="s">
-        <v>110</v>
+        <v>77</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" ht="17.5" spans="1:27">
+      <c r="A2" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="L2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="K2" s="29" t="s">
+      <c r="M2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" s="5"/>
+      <c r="W2" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="X2" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="U2" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="V2" s="5"/>
-      <c r="W2" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="X2" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y2" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z2" s="60" t="s">
-        <v>100</v>
+      <c r="Y2" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" s="55" t="s">
+        <v>107</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>87</v>
+        <v>134</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>94</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" s="28"/>
+        <v>137</v>
+      </c>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="28"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="28"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="28"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -2393,7 +2716,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="26">
         <v>6</v>
       </c>
       <c r="H8">
@@ -2458,130 +2781,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="28"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="28"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="28"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="28"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="28"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="28"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="28"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="28"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="28"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="28"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="28"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="28"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="28"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="28"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="28"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="28"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="28"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="28"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="28"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="28"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="28"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="28"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="28"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="28"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="28"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="28"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="28"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="28"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="28"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="28"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="28"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="28"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="28"/>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="28"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="28"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="28"/>
+      <c r="G44" s="26"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="28"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="28"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="28"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="28"/>
+      <c r="G48" s="26"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="28"/>
+      <c r="G49" s="26"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="28"/>
+      <c r="G50" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2595,21 +2918,21 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A2:B16"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.6380952380952"/>
-    <col min="2" max="2" customWidth="true" width="29.2761904761905"/>
+    <col min="1" max="1" customWidth="true" width="23.6363636363636"/>
+    <col min="2" max="2" customWidth="true" width="29.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>132</v>
+      <c r="A1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2624,72 +2947,72 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.1809523809524" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.2761904761905"/>
-    <col min="2" max="2" customWidth="true" width="23.2761904761905"/>
-    <col min="3" max="3" customWidth="true" width="21.3619047619048"/>
-    <col min="4" max="4" customWidth="true" width="19.1809523809524"/>
-    <col min="5" max="5" customWidth="true" width="12.6380952380952"/>
-    <col min="6" max="6" customWidth="true" width="12.0952380952381"/>
-    <col min="7" max="7" customWidth="true" width="12.1809523809524"/>
-    <col min="8" max="8" customWidth="true" width="46.0952380952381"/>
-    <col min="9" max="16384" customWidth="true" width="19.1809523809524"/>
+    <col min="1" max="1" customWidth="true" width="13.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="23.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="21.3636363636364"/>
+    <col min="4" max="4" customWidth="true" width="19.1818181818182"/>
+    <col min="5" max="5" customWidth="true" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="12.0909090909091"/>
+    <col min="7" max="7" customWidth="true" width="12.1818181818182"/>
+    <col min="8" max="8" customWidth="true" width="46.0909090909091"/>
+    <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" spans="1:8">
-      <c r="A1" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" s="13" t="s">
+    <row r="1" s="9" customFormat="1" spans="1:8">
+      <c r="A1" s="10" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:8">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="10" t="s">
         <v>141</v>
       </c>
+      <c r="C1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" ht="15.5" spans="1:8">
+      <c r="A2" s="55" t="s">
+        <v>148</v>
+      </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="H2" s="62" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2718,20 +3041,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="17.25" spans="7:8">
-      <c r="G6" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" ht="17.25" spans="7:8">
-      <c r="G7" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>152</v>
+    <row r="6" ht="17.5" spans="7:8">
+      <c r="G6" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" ht="17.5" spans="7:8">
+      <c r="G7" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2746,78 +3069,78 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.1809523809524" defaultRowHeight="15" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.2761904761905"/>
-    <col min="2" max="2" customWidth="true" width="23.2761904761905"/>
-    <col min="3" max="3" customWidth="true" width="21.3619047619048"/>
-    <col min="4" max="4" customWidth="true" width="19.1809523809524"/>
-    <col min="5" max="5" customWidth="true" width="12.6380952380952"/>
-    <col min="6" max="6" customWidth="true" width="12.0952380952381"/>
-    <col min="7" max="7" customWidth="true" width="12.1809523809524"/>
-    <col min="8" max="8" customWidth="true" width="46.0952380952381"/>
-    <col min="9" max="16384" customWidth="true" width="19.1809523809524"/>
+    <col min="1" max="1" customWidth="true" width="13.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="23.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="21.3636363636364"/>
+    <col min="4" max="4" customWidth="true" width="19.1818181818182"/>
+    <col min="5" max="5" customWidth="true" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="12.0909090909091"/>
+    <col min="7" max="7" customWidth="true" width="12.1818181818182"/>
+    <col min="8" max="8" customWidth="true" width="46.0909090909091"/>
+    <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" spans="1:9">
-      <c r="A1" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" s="13" t="s">
+    <row r="1" s="9" customFormat="1" spans="1:9">
+      <c r="A1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:9">
+      <c r="B1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" ht="15.5" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="60" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" s="63" t="s">
-        <v>161</v>
+        <v>162</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>168</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="9:9">
@@ -2849,20 +3172,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" ht="17.25" spans="7:8">
-      <c r="G6" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" ht="17.25" spans="7:8">
-      <c r="G7" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>152</v>
+    <row r="6" ht="17.5" spans="7:8">
+      <c r="G6" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" ht="17.5" spans="7:8">
+      <c r="G7" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2874,129 +3197,133 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.0952380952381" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.0952380952381"/>
-    <col min="3" max="3" customWidth="true" width="24.2761904761905"/>
-    <col min="4" max="4" customWidth="true" width="20.0952380952381"/>
-    <col min="5" max="5" customWidth="true" width="24.2761904761905"/>
-    <col min="6" max="6" customWidth="true" width="25.5428571428571"/>
-    <col min="7" max="7" customWidth="true" width="25.2761904761905"/>
-    <col min="8" max="9" customWidth="true" width="20.0952380952381"/>
-    <col min="10" max="10" customWidth="true" width="30.6380952380952"/>
-    <col min="11" max="11" customWidth="true" width="18.5428571428571"/>
-    <col min="12" max="18" customWidth="true" width="20.0952380952381"/>
-    <col min="19" max="19" customWidth="true" width="26.4285714285714"/>
-    <col min="20" max="16384" customWidth="true" width="20.0952380952381"/>
+    <col min="1" max="2" customWidth="true" width="20.0909090909091"/>
+    <col min="3" max="3" customWidth="true" width="24.2727272727273"/>
+    <col min="4" max="4" customWidth="true" width="20.0909090909091"/>
+    <col min="5" max="5" customWidth="true" width="24.2727272727273"/>
+    <col min="6" max="6" customWidth="true" width="25.5454545454545"/>
+    <col min="7" max="7" customWidth="true" width="25.2727272727273"/>
+    <col min="8" max="9" customWidth="true" width="20.0909090909091"/>
+    <col min="10" max="10" customWidth="true" width="30.6363636363636"/>
+    <col min="11" max="11" customWidth="true" width="18.5454545454545"/>
+    <col min="12" max="18" customWidth="true" width="20.0909090909091"/>
+    <col min="19" max="19" customWidth="true" width="26.4272727272727"/>
+    <col min="20" max="20" customWidth="true" width="23.0"/>
+    <col min="21" max="16383" customWidth="true" width="20.0909090909091"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="18" spans="1:19">
+    <row r="1" s="1" customFormat="1" ht="17" spans="1:20">
       <c r="A1" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" ht="90" spans="1:19">
+        <v>187</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" ht="87" spans="1:20">
       <c r="A2" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="6">
-        <v>44938</v>
+        <v>190</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="O2" s="6">
         <v>44938</v>
@@ -3005,13 +3332,16 @@
         <v>1134</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>195</v>
+        <v>14</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3043,32 +3373,32 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.2761904761905"/>
-    <col min="2" max="2" customWidth="true" width="27.3619047619048"/>
-    <col min="3" max="3" customWidth="true" width="14.2761904761905"/>
+    <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="27.3636363636364"/>
+    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="47" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="5"/>
@@ -3085,78 +3415,105 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0"/>
-    <col min="2" max="2" customWidth="true" width="34.0"/>
-    <col min="3" max="16382" customWidth="true" width="18.0"/>
+    <col min="1" max="1" customWidth="true" width="22.8181818181818"/>
+    <col min="2" max="2" customWidth="true" width="21.5454545454545"/>
+    <col min="3" max="3" customWidth="true" width="16.5454545454545"/>
+    <col min="4" max="16382" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="49" t="s">
+      <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>20</v>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>20</v>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:3">
+      <c r="A6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mohamedra" tooltip="mailto:fa@xealei.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="xealei@23"/>
+    <hyperlink ref="C2" r:id="rId1" display="auto@123" tooltip="mailto:auto@123"/>
+    <hyperlink ref="C3" r:id="rId1" display="auto@123" tooltip="mailto:auto@123"/>
+    <hyperlink ref="C4" r:id="rId1" display="auto@123" tooltip="mailto:auto@123"/>
+    <hyperlink ref="C5" r:id="rId1" display="auto@123" tooltip="mailto:auto@123"/>
+    <hyperlink ref="C6" r:id="rId1" display="auto@123" tooltip="mailto:auto@123"/>
+    <hyperlink ref="C7" r:id="rId1" display="auto@123" tooltip="mailto:auto@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3169,80 +3526,84 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6380952380952" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="34" width="12.6380952380952"/>
-    <col min="2" max="2" customWidth="true" style="34" width="28.7238095238095"/>
-    <col min="3" max="5" customWidth="true" style="34" width="12.6380952380952"/>
-    <col min="6" max="6" customWidth="true" width="20.2761904761905"/>
-    <col min="7" max="7" customWidth="true" width="16.8190476190476"/>
-    <col min="8" max="16381" customWidth="true" width="12.6380952380952"/>
+    <col min="1" max="1" customWidth="true" style="32" width="12.6363636363636"/>
+    <col min="2" max="2" customWidth="true" style="32" width="28.7272727272727"/>
+    <col min="3" max="5" customWidth="true" style="32" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
+    <col min="7" max="7" customWidth="true" width="16.8181818181818"/>
+    <col min="8" max="16381" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
-    <row r="1" s="41" customFormat="1" ht="19.5" spans="1:7">
-      <c r="A1" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="36" t="s">
+    <row r="1" s="39" customFormat="1" ht="19.5" spans="1:7">
+      <c r="A1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="B1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:7">
-      <c r="A2" s="44" t="s">
+      <c r="D1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="E1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="F1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="G1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="56" t="s">
+    </row>
+    <row r="2" ht="15.5" spans="1:7">
+      <c r="A2" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="B2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="C2" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="7:7">
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="34">
+      <c r="A6" s="32">
         <v>0</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="32">
         <v>1</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="32">
         <v>2</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="32">
         <v>3</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>4</v>
       </c>
       <c r="F6">
@@ -3264,67 +3625,67 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9047619047619" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7238095238095"/>
-    <col min="2" max="2" customWidth="true" width="32.3619047619048"/>
-    <col min="3" max="5" customWidth="true" style="34" width="12.9047619047619"/>
-    <col min="6" max="6" customWidth="true" width="30.9047619047619"/>
-    <col min="7" max="7" customWidth="true" width="22.2761904761905"/>
-    <col min="8" max="16379" customWidth="true" width="12.9047619047619"/>
+    <col min="1" max="1" customWidth="true" width="21.7272727272727"/>
+    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
+    <col min="3" max="5" customWidth="true" style="32" width="12.9090909090909"/>
+    <col min="6" max="6" customWidth="true" width="30.9090909090909"/>
+    <col min="7" max="7" customWidth="true" width="22.2727272727273"/>
+    <col min="8" max="16379" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
-      <c r="A1" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="A1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" ht="15.5" spans="1:7">
+      <c r="A2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:7">
-      <c r="A2" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>44</v>
+      <c r="D2" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>50</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="34"/>
-      <c r="F3" s="40" t="s">
-        <v>45</v>
+      <c r="B3" s="32"/>
+      <c r="F3" s="38" t="s">
+        <v>51</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -3335,13 +3696,13 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="32">
         <v>2</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="32">
         <v>3</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>4</v>
       </c>
       <c r="F10">
@@ -3360,20 +3721,35 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.9047619047619"/>
+    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
-        <v>46</v>
+      <c r="A1" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3388,21 +3764,21 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B14"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0952380952381"/>
-    <col min="2" max="2" customWidth="true" width="22.4571428571429"/>
+    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
+    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>48</v>
+      <c r="A1" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3416,220 +3792,220 @@
   <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9047619047619" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" customWidth="true" width="21.3619047619048"/>
-    <col min="6" max="6" customWidth="true" width="11.4571428571429"/>
-    <col min="7" max="7" customWidth="true" style="20" width="27.6380952380952"/>
-    <col min="8" max="8" customWidth="true" width="9.36190476190476"/>
-    <col min="9" max="22" customWidth="true" width="21.3619047619048"/>
-    <col min="23" max="23" customWidth="true" width="16.4571428571429"/>
-    <col min="24" max="24" customWidth="true" width="19.7238095238095"/>
-    <col min="25" max="25" customWidth="true" width="21.6380952380952"/>
-    <col min="26" max="26" customWidth="true" width="18.9047619047619"/>
-    <col min="27" max="27" customWidth="true" width="20.5428571428571"/>
-    <col min="28" max="16384" customWidth="true" width="10.9047619047619"/>
+    <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
+    <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
+    <col min="7" max="7" customWidth="true" style="18" width="27.6363636363636"/>
+    <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
+    <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
+    <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
+    <col min="24" max="24" customWidth="true" width="19.7272727272727"/>
+    <col min="25" max="25" customWidth="true" width="21.6363636363636"/>
+    <col min="26" max="26" customWidth="true" width="18.9090909090909"/>
+    <col min="27" max="27" customWidth="true" width="20.5454545454545"/>
+    <col min="28" max="16384" customWidth="true" width="10.9090909090909"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="18" spans="1:27">
-      <c r="A1" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>54</v>
+    <row r="1" s="18" customFormat="1" ht="17" spans="1:27">
+      <c r="A1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="23" t="s">
-        <v>76</v>
+      <c r="A2" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>90</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="30" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>95</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>93</v>
+        <v>99</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="U2" s="59" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+      <c r="U2" s="54" t="s">
+        <v>103</v>
       </c>
       <c r="V2" s="5"/>
-      <c r="W2" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="X2" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y2" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z2" s="60" t="s">
-        <v>100</v>
+      <c r="W2" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y2" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" s="55" t="s">
+        <v>107</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="28"/>
+        <v>114</v>
+      </c>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="28"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="28"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="28"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -3650,7 +4026,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="26">
         <v>6</v>
       </c>
       <c r="H8">
@@ -3715,130 +4091,130 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="28"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="28"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="28"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="28"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="28"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="28"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="28"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="28"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="28"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="28"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="28"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="28"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="28"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="28"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="28"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="28"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="28"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="28"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="28"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="28"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="28"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="28"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="28"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="28"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="28"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="28"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="28"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="28"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="28"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="28"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="28"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="28"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="28"/>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="28"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="28"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="28"/>
+      <c r="G44" s="26"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="28"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="28"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="28"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="28"/>
+      <c r="G48" s="26"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="28"/>
+      <c r="G49" s="26"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="28"/>
+      <c r="G50" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3852,25 +4228,25 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="A2:C17"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.2761904761905"/>
-    <col min="2" max="2" customWidth="true" width="20.6380952380952"/>
-    <col min="3" max="3" customWidth="true" width="11.1809523809524"/>
+    <col min="1" max="1" customWidth="true" width="19.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="20.6363636363636"/>
+    <col min="3" max="3" customWidth="true" width="11.1818181818182"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>109</v>
+      <c r="A1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upto Notification Date field
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="308">
   <si>
     <t>Environment Name</t>
   </si>
@@ -1182,6 +1182,60 @@
   </si>
   <si>
     <t>01/11/202406:47PM</t>
+  </si>
+  <si>
+    <t>01/12/202412:13PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-13:32</t>
+  </si>
+  <si>
+    <t>01/12/202412:17PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-17:52</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-21:24</t>
+  </si>
+  <si>
+    <t>01/12/202412:21PM</t>
+  </si>
+  <si>
+    <t>01/12/202401:18PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-18:18</t>
+  </si>
+  <si>
+    <t>01/12/202402:10PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-10:24</t>
+  </si>
+  <si>
+    <t>01/12/202402:18PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-18:40</t>
+  </si>
+  <si>
+    <t>01/12/202402:40PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-40:38</t>
+  </si>
+  <si>
+    <t>01/12/202402:41PM</t>
+  </si>
+  <si>
+    <t>01/12/202402:47PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-47:27</t>
+  </si>
+  <si>
+    <t>01/12/202402:48PM</t>
   </si>
 </sst>
 </file>
@@ -3287,7 +3341,7 @@
         <v>190</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>192</v>
@@ -3338,7 +3392,7 @@
         <v>14</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="T2" s="55" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
Rejection by residential manager code added.
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="276">
   <si>
     <t>Environment Name</t>
   </si>
@@ -885,6 +885,189 @@
   </si>
   <si>
     <t>IR00070</t>
+  </si>
+  <si>
+    <t>test - -07:21</t>
+  </si>
+  <si>
+    <t>IR00075</t>
+  </si>
+  <si>
+    <t>test - -08:55</t>
+  </si>
+  <si>
+    <t>IR00076</t>
+  </si>
+  <si>
+    <t>test - -11:05</t>
+  </si>
+  <si>
+    <t>IR00077</t>
+  </si>
+  <si>
+    <t>test - -20:39</t>
+  </si>
+  <si>
+    <t>IR00078</t>
+  </si>
+  <si>
+    <t>test - -22:32</t>
+  </si>
+  <si>
+    <t>IR00079</t>
+  </si>
+  <si>
+    <t>test - -35:44</t>
+  </si>
+  <si>
+    <t>IR00082</t>
+  </si>
+  <si>
+    <t>test - -48:11</t>
+  </si>
+  <si>
+    <t>IR00083</t>
+  </si>
+  <si>
+    <t>test - -02:04</t>
+  </si>
+  <si>
+    <t>IR00084</t>
+  </si>
+  <si>
+    <t>test - -19:06</t>
+  </si>
+  <si>
+    <t>IR00085</t>
+  </si>
+  <si>
+    <t>test - -21:42</t>
+  </si>
+  <si>
+    <t>IR00086</t>
+  </si>
+  <si>
+    <t>test - -24:38</t>
+  </si>
+  <si>
+    <t>IR00087</t>
+  </si>
+  <si>
+    <t>test - -46:02</t>
+  </si>
+  <si>
+    <t>IR00088</t>
+  </si>
+  <si>
+    <t>test - -25:00</t>
+  </si>
+  <si>
+    <t>IR00089</t>
+  </si>
+  <si>
+    <t>test - -34:55</t>
+  </si>
+  <si>
+    <t>IR00090</t>
+  </si>
+  <si>
+    <t>test - -37:48</t>
+  </si>
+  <si>
+    <t>IR00091</t>
+  </si>
+  <si>
+    <t>test - -23:55</t>
+  </si>
+  <si>
+    <t>IR00093</t>
+  </si>
+  <si>
+    <t>test - -26:11</t>
+  </si>
+  <si>
+    <t>IR00094</t>
+  </si>
+  <si>
+    <t>test - -30:42</t>
+  </si>
+  <si>
+    <t>IR00095</t>
+  </si>
+  <si>
+    <t>test - -55:19</t>
+  </si>
+  <si>
+    <t>test - -15:52</t>
+  </si>
+  <si>
+    <t>IR00112</t>
+  </si>
+  <si>
+    <t>test - -17:51</t>
+  </si>
+  <si>
+    <t>IR00113</t>
+  </si>
+  <si>
+    <t>test - -45:11</t>
+  </si>
+  <si>
+    <t>IR00142</t>
+  </si>
+  <si>
+    <t>test - -04:05</t>
+  </si>
+  <si>
+    <t>IR00143</t>
+  </si>
+  <si>
+    <t>test - -05:22</t>
+  </si>
+  <si>
+    <t>IR00144</t>
+  </si>
+  <si>
+    <t>test - -13:45</t>
+  </si>
+  <si>
+    <t>IR00145</t>
+  </si>
+  <si>
+    <t>test - -48:45</t>
+  </si>
+  <si>
+    <t>IR00146</t>
+  </si>
+  <si>
+    <t>test - -58:49</t>
+  </si>
+  <si>
+    <t>IR00147</t>
+  </si>
+  <si>
+    <t>test - -06:53</t>
+  </si>
+  <si>
+    <t>IR00148</t>
+  </si>
+  <si>
+    <t>test - -11:06</t>
+  </si>
+  <si>
+    <t>IR00149</t>
+  </si>
+  <si>
+    <t>test - -18:44</t>
+  </si>
+  <si>
+    <t>IR00150</t>
+  </si>
+  <si>
+    <t>test - -34:21</t>
+  </si>
+  <si>
+    <t>IR00151</t>
   </si>
 </sst>
 </file>
@@ -3100,10 +3283,10 @@
         <v>14</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>213</v>
+        <v>274</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>214</v>
+        <v>275</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>205</v>

</xml_diff>

<commit_message>
updated testscripts for Login Module
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="10" activeTab="13"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="236">
   <si>
     <t>Environment Name</t>
   </si>
@@ -80,6 +80,9 @@
     <t>Location</t>
   </si>
   <si>
+    <t>Login Names</t>
+  </si>
+  <si>
     <t>FACILITY ADMIN</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
     <t>ATFacilityAdmin</t>
   </si>
   <si>
+    <t>Staff</t>
+  </si>
+  <si>
     <t>STAFF</t>
   </si>
   <si>
@@ -104,22 +110,34 @@
     <t>AChief_Nu</t>
   </si>
   <si>
+    <t>Chief Nurse</t>
+  </si>
+  <si>
     <t>RESIDENT MANAGER</t>
   </si>
   <si>
     <t>AManager</t>
   </si>
   <si>
+    <t>Resident Manager</t>
+  </si>
+  <si>
     <t>CLINICAL COORDINATOR</t>
   </si>
   <si>
     <t>AClinical</t>
   </si>
   <si>
+    <t>Clinical Coordinator</t>
+  </si>
+  <si>
     <t>SOCIAL WORKER</t>
   </si>
   <si>
     <t>ASWorker</t>
+  </si>
+  <si>
+    <t>Social Worker</t>
   </si>
   <si>
     <t>SuiteName*</t>
@@ -800,7 +818,7 @@
     <t>Arlia Thomas</t>
   </si>
   <si>
-    <t>01/18/202408:53PM</t>
+    <t>01/22/202403:16PM</t>
   </si>
   <si>
     <t>Low BP</t>
@@ -833,19 +851,19 @@
     <t>John Smith</t>
   </si>
   <si>
-    <t>1/18/2024</t>
-  </si>
-  <si>
-    <t>08:54PM</t>
+    <t>1/22/2024</t>
+  </si>
+  <si>
+    <t>03:16PM</t>
   </si>
   <si>
     <t>Jane Doe</t>
   </si>
   <si>
-    <t>Twisted Ankle-54:03</t>
-  </si>
-  <si>
-    <t>IR00125</t>
+    <t>Twisted Ankle-16:14</t>
+  </si>
+  <si>
+    <t>IR00163</t>
   </si>
   <si>
     <t>Chief nurse approved.</t>
@@ -872,160 +890,28 @@
     <t>Social Worker rejected.</t>
   </si>
   <si>
-    <t>01/18/202409:02PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-02:53</t>
-  </si>
-  <si>
-    <t>01/18/202409:06PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-06:29</t>
-  </si>
-  <si>
-    <t>01/18/202409:09PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-09:49</t>
-  </si>
-  <si>
-    <t>01/18/202409:10PM</t>
-  </si>
-  <si>
-    <t>09:10PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-10:47</t>
-  </si>
-  <si>
-    <t>01/18/202409:30PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-30:44</t>
-  </si>
-  <si>
-    <t>01/18/202409:31PM</t>
-  </si>
-  <si>
-    <t>09:31PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-31:42</t>
-  </si>
-  <si>
-    <t>01/18/202409:40PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-40:51</t>
-  </si>
-  <si>
-    <t>01/18/202409:41PM</t>
-  </si>
-  <si>
-    <t>09:41PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-41:50</t>
-  </si>
-  <si>
-    <t>01/19/202404:48PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-48:38</t>
-  </si>
-  <si>
-    <t>1/19/2024</t>
-  </si>
-  <si>
-    <t>04:48PM</t>
-  </si>
-  <si>
-    <t>IR00152</t>
-  </si>
-  <si>
-    <t>01/19/202404:53PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-53:48</t>
-  </si>
-  <si>
-    <t>04:53PM</t>
-  </si>
-  <si>
-    <t>IR00153</t>
-  </si>
-  <si>
-    <t>01/19/202404:56PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-56:30</t>
-  </si>
-  <si>
-    <t>04:56PM</t>
-  </si>
-  <si>
-    <t>IR00154</t>
-  </si>
-  <si>
-    <t>01/19/202405:02PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-02:08</t>
-  </si>
-  <si>
-    <t>05:02PM</t>
-  </si>
-  <si>
-    <t>IR00155</t>
-  </si>
-  <si>
-    <t>01/19/202405:06PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-06:45</t>
-  </si>
-  <si>
-    <t>05:06PM</t>
-  </si>
-  <si>
-    <t>IR00156</t>
-  </si>
-  <si>
-    <t>01/19/202405:10PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-10:33</t>
-  </si>
-  <si>
-    <t>05:10PM</t>
-  </si>
-  <si>
-    <t>IR00157</t>
-  </si>
-  <si>
-    <t>01/19/202405:13PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-13:27</t>
-  </si>
-  <si>
-    <t>05:13PM</t>
-  </si>
-  <si>
-    <t>IR00158</t>
-  </si>
-  <si>
-    <t>01/19/202405:16PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-16:28</t>
-  </si>
-  <si>
-    <t>05:16PM</t>
-  </si>
-  <si>
-    <t>IR00159</t>
+    <t>01/22/202403:36PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-36:38</t>
+  </si>
+  <si>
+    <t>03:36PM</t>
+  </si>
+  <si>
+    <t>IR00177</t>
+  </si>
+  <si>
+    <t>01/22/202403:40PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-41:06</t>
+  </si>
+  <si>
+    <t>03:41PM</t>
+  </si>
+  <si>
+    <t>IR00178</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1727,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1923,12 +1809,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2294,31 +2182,31 @@
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="56" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="55" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="56" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2359,188 +2247,188 @@
   <sheetData>
     <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="20" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" ht="17.5" spans="1:27">
       <c r="A2" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="L2" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K2" s="28" t="s">
+      <c r="M2" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="U2" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="V2" s="6"/>
+      <c r="W2" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="X2" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="Y2" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="S2" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="U2" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="X2" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y2" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z2" s="59" t="s">
-        <v>105</v>
+      <c r="Z2" s="61" t="s">
+        <v>111</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="6" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="G4" s="27"/>
     </row>
@@ -2785,10 +2673,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2821,54 +2709,54 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:8">
       <c r="A1" s="11" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="59" t="s">
-        <v>146</v>
+      <c r="A2" s="61" t="s">
+        <v>152</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>152</v>
-      </c>
-      <c r="H2" s="61" t="s">
         <v>153</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="63" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2899,18 +2787,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2943,60 +2831,60 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:9">
       <c r="A1" s="11" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
       <c r="A2" s="6" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="62" t="s">
         <v>166</v>
       </c>
+      <c r="C2" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>172</v>
+      </c>
       <c r="I2" s="6" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="9:9">
@@ -3030,18 +2918,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3055,8 +2943,8 @@
   <sheetPr/>
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5"/>
@@ -3084,180 +2972,180 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17" spans="1:29">
       <c r="A1" s="3" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" ht="101.5" spans="1:29">
       <c r="A2" s="6" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:29">
@@ -3385,10 +3273,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="6"/>
@@ -3405,20 +3293,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0"/>
+    <col min="1" max="1" customWidth="true" width="22.5454545454545"/>
     <col min="2" max="2" customWidth="true" width="34.0"/>
     <col min="3" max="16382" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="46" t="s">
         <v>13</v>
       </c>
@@ -3431,80 +3319,111 @@
       <c r="D1" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="47" t="s">
+      <c r="E1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="47" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="B2" s="48" t="s">
         <v>19</v>
       </c>
+      <c r="C2" s="49" t="s">
+        <v>20</v>
+      </c>
       <c r="D2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="49" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="47" t="s">
+      <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="E3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="47" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="47" t="s">
+      <c r="C4" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="47" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="C5" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3541,45 +3460,45 @@
   <sheetData>
     <row r="1" s="40" customFormat="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="43" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="55" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>47</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G2" s="6"/>
     </row>
@@ -3636,52 +3555,52 @@
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>48</v>
+      <c r="D2" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>54</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G3" s="6"/>
     </row>
@@ -3730,7 +3649,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="12" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3756,10 +3675,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="32" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3794,188 +3713,188 @@
   <sheetData>
     <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="20" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="22" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>92</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="U2" s="58" t="s">
-        <v>101</v>
+        <v>106</v>
+      </c>
+      <c r="U2" s="60" t="s">
+        <v>107</v>
       </c>
       <c r="V2" s="6"/>
-      <c r="W2" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="X2" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y2" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z2" s="59" t="s">
-        <v>105</v>
+      <c r="W2" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="X2" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y2" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z2" s="61" t="s">
+        <v>111</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G4" s="27"/>
     </row>
@@ -4221,13 +4140,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot Password Test scripts
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,30 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="18350" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
     <sheet name="URL" sheetId="5" r:id="rId2"/>
     <sheet name="Login" sheetId="2" r:id="rId3"/>
-    <sheet name="AddSuites" sheetId="3" r:id="rId4"/>
-    <sheet name="EditSuites" sheetId="4" r:id="rId5"/>
-    <sheet name="CreatedSuites" sheetId="6" r:id="rId6"/>
-    <sheet name="UpdatedSuites" sheetId="7" r:id="rId7"/>
-    <sheet name="AddIndividuals" sheetId="8" r:id="rId8"/>
-    <sheet name="CreatedIndividuals" sheetId="9" r:id="rId9"/>
-    <sheet name="EditIndividuals" sheetId="10" r:id="rId10"/>
-    <sheet name="UpdatedIndividuals" sheetId="14" r:id="rId11"/>
-    <sheet name="AddVitals" sheetId="11" r:id="rId12"/>
-    <sheet name="EditVitals" sheetId="13" r:id="rId13"/>
-    <sheet name="Incident Reports" sheetId="15" r:id="rId14"/>
+    <sheet name="Forgot Password" sheetId="16" r:id="rId4"/>
+    <sheet name="AddSuites" sheetId="3" r:id="rId5"/>
+    <sheet name="EditSuites" sheetId="4" r:id="rId6"/>
+    <sheet name="CreatedSuites" sheetId="6" r:id="rId7"/>
+    <sheet name="UpdatedSuites" sheetId="7" r:id="rId8"/>
+    <sheet name="AddIndividuals" sheetId="8" r:id="rId9"/>
+    <sheet name="CreatedIndividuals" sheetId="9" r:id="rId10"/>
+    <sheet name="EditIndividuals" sheetId="10" r:id="rId11"/>
+    <sheet name="UpdatedIndividuals" sheetId="14" r:id="rId12"/>
+    <sheet name="AddVitals" sheetId="11" r:id="rId13"/>
+    <sheet name="EditVitals" sheetId="13" r:id="rId14"/>
+    <sheet name="Incident Reports" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="236">
   <si>
     <t>Environment Name</t>
   </si>
@@ -59,15 +60,12 @@
     <t>Login Page</t>
   </si>
   <si>
-    <t>Suite Page</t>
+    <t>Forgot Password Page</t>
   </si>
   <si>
     <t>assets/img/xealei-logo2.png</t>
   </si>
   <si>
-    <t>https://gha.qa.xealei.com/login</t>
-  </si>
-  <si>
     <t>Names</t>
   </si>
   <si>
@@ -138,6 +136,33 @@
   </si>
   <si>
     <t>Social Worker</t>
+  </si>
+  <si>
+    <t>Invalid Email formats</t>
+  </si>
+  <si>
+    <t>UnRegistered Email</t>
+  </si>
+  <si>
+    <t>Blocked Email</t>
+  </si>
+  <si>
+    <t>In-Active Email</t>
+  </si>
+  <si>
+    <t>anjelaJ</t>
+  </si>
+  <si>
+    <t>mohamedrazul.s@gmail.com</t>
+  </si>
+  <si>
+    <t>mohamedrazul.s+1@alphind.com</t>
+  </si>
+  <si>
+    <t>anjelaJ@Gha</t>
+  </si>
+  <si>
+    <t>123@g.in</t>
   </si>
   <si>
     <t>SuiteName*</t>
@@ -818,7 +843,7 @@
     <t>Arlia Thomas</t>
   </si>
   <si>
-    <t>01/22/202403:16PM</t>
+    <t>01/22/202403:40PM</t>
   </si>
   <si>
     <t>Low BP</t>
@@ -854,16 +879,16 @@
     <t>1/22/2024</t>
   </si>
   <si>
-    <t>03:16PM</t>
+    <t>03:41PM</t>
   </si>
   <si>
     <t>Jane Doe</t>
   </si>
   <si>
-    <t>Twisted Ankle-16:14</t>
-  </si>
-  <si>
-    <t>IR00163</t>
+    <t>Twisted Ankle-41:06</t>
+  </si>
+  <si>
+    <t>IR00178</t>
   </si>
   <si>
     <t>Chief nurse approved.</t>
@@ -888,30 +913,6 @@
   </si>
   <si>
     <t>Social Worker rejected.</t>
-  </si>
-  <si>
-    <t>01/22/202403:36PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-36:38</t>
-  </si>
-  <si>
-    <t>03:36PM</t>
-  </si>
-  <si>
-    <t>IR00177</t>
-  </si>
-  <si>
-    <t>01/22/202403:40PM</t>
-  </si>
-  <si>
-    <t>Twisted Ankle-41:06</t>
-  </si>
-  <si>
-    <t>03:41PM</t>
-  </si>
-  <si>
-    <t>IR00178</t>
   </si>
 </sst>
 </file>
@@ -925,7 +926,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1054,6 +1055,13 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1597,137 +1605,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1809,19 +1817,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1831,6 +1839,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1839,7 +1849,6 @@
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2169,13 +2178,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.3636363636364"/>
-    <col min="2" max="2" customWidth="true" width="29.0909090909091"/>
+    <col min="1" max="1" width="17.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="29.0909090909091" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2224,6 +2233,39 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="A2:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="19.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="20.6363636363636" customWidth="1"/>
+    <col min="3" max="3" width="11.1818181818182" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
@@ -2232,203 +2274,203 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
-    <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
-    <col min="7" max="7" customWidth="true" style="19" width="27.6363636363636"/>
-    <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
-    <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
-    <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
-    <col min="24" max="24" customWidth="true" width="19.7272727272727"/>
-    <col min="25" max="25" customWidth="true" width="21.6363636363636"/>
-    <col min="26" max="26" customWidth="true" width="18.9090909090909"/>
-    <col min="27" max="27" customWidth="true" width="20.5454545454545"/>
-    <col min="28" max="16383" customWidth="true" width="10.9090909090909"/>
+    <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
+    <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
+    <col min="7" max="7" width="27.6363636363636" style="19" customWidth="1"/>
+    <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
+    <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
+    <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
+    <col min="24" max="24" width="19.7272727272727" customWidth="1"/>
+    <col min="25" max="25" width="21.6363636363636" customWidth="1"/>
+    <col min="26" max="26" width="18.9090909090909" customWidth="1"/>
+    <col min="27" max="27" width="20.5454545454545" customWidth="1"/>
+    <col min="28" max="16383" width="10.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="20" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" ht="17.5" spans="1:27">
       <c r="A2" s="22" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="L2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="K2" s="28" t="s">
+      <c r="M2" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="U2" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="V2" s="6"/>
+      <c r="W2" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="R2" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="S2" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="U2" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="X2" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y2" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z2" s="61" t="s">
-        <v>111</v>
+      <c r="X2" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z2" s="57" t="s">
+        <v>119</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="6" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="6" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="G4" s="27"/>
     </row>
@@ -2656,7 +2698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B1"/>
@@ -2667,16 +2709,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.6363636363636"/>
-    <col min="2" max="2" customWidth="true" width="29.2727272727273"/>
+    <col min="1" max="1" width="23.6363636363636" customWidth="1"/>
+    <col min="2" max="2" width="29.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2685,7 +2727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H7"/>
@@ -2696,67 +2738,67 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.2727272727273"/>
-    <col min="2" max="2" customWidth="true" width="23.2727272727273"/>
-    <col min="3" max="3" customWidth="true" width="21.3636363636364"/>
-    <col min="4" max="4" customWidth="true" width="19.1818181818182"/>
-    <col min="5" max="5" customWidth="true" width="12.6363636363636"/>
-    <col min="6" max="6" customWidth="true" width="12.0909090909091"/>
-    <col min="7" max="7" customWidth="true" width="12.1818181818182"/>
-    <col min="8" max="8" customWidth="true" width="46.0909090909091"/>
-    <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
+    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="23.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="21.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="19.1818181818182" customWidth="1"/>
+    <col min="5" max="5" width="12.6363636363636" customWidth="1"/>
+    <col min="6" max="6" width="12.0909090909091" customWidth="1"/>
+    <col min="7" max="7" width="12.1818181818182" customWidth="1"/>
+    <col min="8" max="8" width="46.0909090909091" customWidth="1"/>
+    <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:8">
       <c r="A1" s="11" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="61" t="s">
-        <v>152</v>
+      <c r="A2" s="57" t="s">
+        <v>160</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>156</v>
-      </c>
-      <c r="F2" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="63" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2787,18 +2829,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2807,7 +2849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I7"/>
@@ -2818,73 +2860,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.2727272727273"/>
-    <col min="2" max="2" customWidth="true" width="23.2727272727273"/>
-    <col min="3" max="3" customWidth="true" width="21.3636363636364"/>
-    <col min="4" max="4" customWidth="true" width="19.1818181818182"/>
-    <col min="5" max="5" customWidth="true" width="12.6363636363636"/>
-    <col min="6" max="6" customWidth="true" width="12.0909090909091"/>
-    <col min="7" max="7" customWidth="true" width="12.1818181818182"/>
-    <col min="8" max="8" customWidth="true" width="46.0909090909091"/>
-    <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
+    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="23.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="21.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="19.1818181818182" customWidth="1"/>
+    <col min="5" max="5" width="12.6363636363636" customWidth="1"/>
+    <col min="6" max="6" width="12.0909090909091" customWidth="1"/>
+    <col min="7" max="7" width="12.1818181818182" customWidth="1"/>
+    <col min="8" max="8" width="46.0909090909091" customWidth="1"/>
+    <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:9">
       <c r="A1" s="11" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
       <c r="A2" s="6" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="61" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>180</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="9:9">
@@ -2918,18 +2960,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2938,7 +2980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AC11"/>
@@ -2949,203 +2991,203 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.0909090909091"/>
-    <col min="3" max="3" customWidth="true" width="24.2727272727273"/>
-    <col min="4" max="4" customWidth="true" width="20.0909090909091"/>
-    <col min="5" max="5" customWidth="true" width="24.2727272727273"/>
-    <col min="6" max="6" customWidth="true" width="25.5454545454545"/>
-    <col min="7" max="7" customWidth="true" width="25.2727272727273"/>
-    <col min="8" max="9" customWidth="true" width="20.0909090909091"/>
-    <col min="10" max="10" customWidth="true" width="30.6363636363636"/>
-    <col min="11" max="11" customWidth="true" width="18.5454545454545"/>
-    <col min="12" max="18" customWidth="true" width="20.0909090909091"/>
-    <col min="19" max="19" customWidth="true" width="26.4272727272727"/>
-    <col min="20" max="20" customWidth="true" width="22.1454545454545"/>
-    <col min="21" max="21" customWidth="true" width="47.1454545454545"/>
-    <col min="22" max="23" customWidth="true" width="54.7181818181818"/>
-    <col min="24" max="24" customWidth="true" width="47.1454545454545"/>
-    <col min="25" max="25" customWidth="true" width="44.8545454545455"/>
-    <col min="26" max="27" customWidth="true" width="55.0"/>
-    <col min="28" max="28" customWidth="true" width="46.7181818181818"/>
-    <col min="29" max="16384" customWidth="true" width="20.0909090909091"/>
+    <col min="1" max="2" width="20.0909090909091" customWidth="1"/>
+    <col min="3" max="3" width="24.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="20.0909090909091" customWidth="1"/>
+    <col min="5" max="5" width="24.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="25.5454545454545" customWidth="1"/>
+    <col min="7" max="7" width="25.2727272727273" customWidth="1"/>
+    <col min="8" max="9" width="20.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="30.6363636363636" customWidth="1"/>
+    <col min="11" max="11" width="18.5454545454545" customWidth="1"/>
+    <col min="12" max="18" width="20.0909090909091" customWidth="1"/>
+    <col min="19" max="19" width="26.4272727272727" customWidth="1"/>
+    <col min="20" max="20" width="22.1454545454545" customWidth="1"/>
+    <col min="21" max="21" width="47.1454545454545" customWidth="1"/>
+    <col min="22" max="23" width="54.7181818181818" customWidth="1"/>
+    <col min="24" max="24" width="47.1454545454545" customWidth="1"/>
+    <col min="25" max="25" width="44.8545454545455" customWidth="1"/>
+    <col min="26" max="27" width="55" customWidth="1"/>
+    <col min="28" max="28" width="46.7181818181818" customWidth="1"/>
+    <col min="29" max="16384" width="20.0909090909091" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17" spans="1:29">
       <c r="A1" s="3" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" ht="101.5" spans="1:29">
       <c r="A2" s="6" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="Z2" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:29">
@@ -3251,14 +3293,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
-    <col min="2" max="2" customWidth="true" width="27.3636363636364"/>
-    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
+    <col min="1" max="1" width="31.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="27.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="23.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3273,17 +3315,19 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="6"/>
+      <c r="B2" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://gha.qa.xealei.com/login"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://xat.qa.xealei.com/" tooltip="https://xat.qa.xealei.com/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3295,134 +3339,134 @@
   <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.5454545454545"/>
-    <col min="2" max="2" customWidth="true" width="34.0"/>
-    <col min="3" max="16382" customWidth="true" width="18.0"/>
+    <col min="1" max="1" width="22.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="16382" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="C1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="47" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="50" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="48" t="s">
+      <c r="B2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="C2" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="50" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="50" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="C3" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="B4" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="51" t="s">
+      <c r="E4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="49" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="48" t="s">
+      <c r="E5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="49" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="48" t="s">
+      <c r="E6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="49" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="48" t="s">
+      <c r="E7" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3442,6 +3486,74 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="19.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="26.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="17.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="24.2727272727273" customWidth="1"/>
+    <col min="5" max="5" width="33.4545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="mohamedrazul.s@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="123@g.in"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3450,55 +3562,55 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="33" width="12.6363636363636"/>
-    <col min="2" max="2" customWidth="true" style="33" width="28.7272727272727"/>
-    <col min="3" max="5" customWidth="true" style="33" width="12.6363636363636"/>
-    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
-    <col min="7" max="7" customWidth="true" width="16.8181818181818"/>
-    <col min="8" max="16381" customWidth="true" width="12.6363636363636"/>
+    <col min="1" max="1" width="12.6363636363636" style="33" customWidth="1"/>
+    <col min="2" max="2" width="28.7272727272727" style="33" customWidth="1"/>
+    <col min="3" max="5" width="12.6363636363636" style="33" customWidth="1"/>
+    <col min="6" max="6" width="20.2727272727273" customWidth="1"/>
+    <col min="7" max="7" width="16.8181818181818" customWidth="1"/>
+    <col min="8" max="16381" width="12.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="40" customFormat="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="43" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>55</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G2" s="6"/>
     </row>
@@ -3534,7 +3646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G10"/>
@@ -3545,62 +3657,62 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7272727272727"/>
-    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
-    <col min="3" max="5" customWidth="true" style="33" width="12.9090909090909"/>
-    <col min="6" max="6" customWidth="true" width="30.9090909090909"/>
-    <col min="7" max="7" customWidth="true" width="22.2727272727273"/>
-    <col min="8" max="16379" customWidth="true" width="12.9090909090909"/>
+    <col min="1" max="1" width="21.7272727272727" customWidth="1"/>
+    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
+    <col min="3" max="5" width="12.9090909090909" style="33" customWidth="1"/>
+    <col min="6" max="6" width="30.9090909090909" customWidth="1"/>
+    <col min="7" max="7" width="22.2727272727273" customWidth="1"/>
+    <col min="8" max="16379" width="12.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="58" t="s">
+      <c r="C2" s="60" t="s">
         <v>54</v>
       </c>
+      <c r="D2" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="60" t="s">
+        <v>62</v>
+      </c>
       <c r="F2" s="37" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G3" s="6"/>
     </row>
@@ -3633,7 +3745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1"/>
@@ -3644,12 +3756,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
+    <col min="1" max="1" width="22.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="12" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3658,7 +3770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B1"/>
@@ -3669,16 +3781,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
-    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
+    <col min="1" max="1" width="18.0909090909091" customWidth="1"/>
+    <col min="2" max="2" width="22.4545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="32" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3687,7 +3799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AA50"/>
@@ -3698,203 +3810,203 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
-    <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
-    <col min="7" max="7" customWidth="true" style="19" width="27.6363636363636"/>
-    <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
-    <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
-    <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
-    <col min="24" max="24" customWidth="true" width="19.7272727272727"/>
-    <col min="25" max="25" customWidth="true" width="21.6363636363636"/>
-    <col min="26" max="26" customWidth="true" width="18.9090909090909"/>
-    <col min="27" max="27" customWidth="true" width="20.5454545454545"/>
-    <col min="28" max="16384" customWidth="true" width="10.9090909090909"/>
+    <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
+    <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
+    <col min="7" max="7" width="27.6363636363636" style="19" customWidth="1"/>
+    <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
+    <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
+    <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
+    <col min="24" max="24" width="19.7272727272727" customWidth="1"/>
+    <col min="25" max="25" width="21.6363636363636" customWidth="1"/>
+    <col min="26" max="26" width="18.9090909090909" customWidth="1"/>
+    <col min="27" max="27" width="20.5454545454545" customWidth="1"/>
+    <col min="28" max="16384" width="10.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="20" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="22" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>92</v>
+        <v>99</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>100</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="U2" s="60" t="s">
-        <v>107</v>
+        <v>114</v>
+      </c>
+      <c r="U2" s="62" t="s">
+        <v>115</v>
       </c>
       <c r="V2" s="6"/>
-      <c r="W2" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="X2" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y2" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z2" s="61" t="s">
-        <v>111</v>
+      <c r="W2" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="X2" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z2" s="57" t="s">
+        <v>119</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="6" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G4" s="27"/>
     </row>
@@ -4115,39 +4227,6 @@
     </row>
     <row r="50" spans="7:7">
       <c r="G50" s="27"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="A2:C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="19.2727272727273"/>
-    <col min="2" max="2" customWidth="true" width="20.6363636363636"/>
-    <col min="3" max="3" customWidth="true" width="11.1818181818182"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>120</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Select - IR Notification
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,31 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="6" activeTab="8"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
     <sheet name="URL" sheetId="5" r:id="rId2"/>
     <sheet name="Login" sheetId="2" r:id="rId3"/>
-    <sheet name="Forgot Password" sheetId="16" r:id="rId4"/>
-    <sheet name="AddSuites" sheetId="3" r:id="rId5"/>
-    <sheet name="EditSuites" sheetId="4" r:id="rId6"/>
-    <sheet name="CreatedSuites" sheetId="6" r:id="rId7"/>
-    <sheet name="UpdatedSuites" sheetId="7" r:id="rId8"/>
-    <sheet name="AddIndividuals" sheetId="8" r:id="rId9"/>
-    <sheet name="CreatedIndividuals" sheetId="9" r:id="rId10"/>
-    <sheet name="EditIndividuals" sheetId="10" r:id="rId11"/>
-    <sheet name="UpdatedIndividuals" sheetId="14" r:id="rId12"/>
-    <sheet name="AddVitals" sheetId="11" r:id="rId13"/>
-    <sheet name="EditVitals" sheetId="13" r:id="rId14"/>
-    <sheet name="Incident Reports" sheetId="15" r:id="rId15"/>
+    <sheet name="AddSuites" sheetId="3" r:id="rId4"/>
+    <sheet name="EditSuites" sheetId="4" r:id="rId5"/>
+    <sheet name="CreatedSuites" sheetId="6" r:id="rId6"/>
+    <sheet name="UpdatedSuites" sheetId="7" r:id="rId7"/>
+    <sheet name="AddIndividuals" sheetId="8" r:id="rId8"/>
+    <sheet name="CreatedIndividuals" sheetId="9" r:id="rId9"/>
+    <sheet name="EditIndividuals" sheetId="10" r:id="rId10"/>
+    <sheet name="UpdatedIndividuals" sheetId="14" r:id="rId11"/>
+    <sheet name="AddVitals" sheetId="11" r:id="rId12"/>
+    <sheet name="EditVitals" sheetId="13" r:id="rId13"/>
+    <sheet name="Incident Reports" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="234">
   <si>
     <t>Environment Name</t>
   </si>
@@ -60,12 +59,15 @@
     <t>Login Page</t>
   </si>
   <si>
-    <t>Forgot Password Page</t>
+    <t>Suite Page</t>
   </si>
   <si>
     <t>assets/img/xealei-logo2.png</t>
   </si>
   <si>
+    <t>https://gha.qa.xealei.com/login</t>
+  </si>
+  <si>
     <t>Names</t>
   </si>
   <si>
@@ -78,9 +80,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Login Names</t>
-  </si>
-  <si>
     <t>FACILITY ADMIN</t>
   </si>
   <si>
@@ -93,9 +92,6 @@
     <t>ATFacilityAdmin</t>
   </si>
   <si>
-    <t>Staff</t>
-  </si>
-  <si>
     <t>STAFF</t>
   </si>
   <si>
@@ -108,63 +104,24 @@
     <t>AChief_Nu</t>
   </si>
   <si>
-    <t>Chief Nurse</t>
-  </si>
-  <si>
     <t>RESIDENT MANAGER</t>
   </si>
   <si>
     <t>AManager</t>
   </si>
   <si>
-    <t>Resident Manager</t>
-  </si>
-  <si>
     <t>CLINICAL COORDINATOR</t>
   </si>
   <si>
     <t>AClinical</t>
   </si>
   <si>
-    <t>Clinical Coordinator</t>
-  </si>
-  <si>
     <t>SOCIAL WORKER</t>
   </si>
   <si>
     <t>ASWorker</t>
   </si>
   <si>
-    <t>Social Worker</t>
-  </si>
-  <si>
-    <t>Invalid Email formats</t>
-  </si>
-  <si>
-    <t>UnRegistered Email</t>
-  </si>
-  <si>
-    <t>Blocked Email</t>
-  </si>
-  <si>
-    <t>In-Active Email</t>
-  </si>
-  <si>
-    <t>anjelaJ</t>
-  </si>
-  <si>
-    <t>mohamedrazul.s@gmail.com</t>
-  </si>
-  <si>
-    <t>mohamedrazul.s+1@alphind.com</t>
-  </si>
-  <si>
-    <t>anjelaJ@Gha</t>
-  </si>
-  <si>
-    <t>123@g.in</t>
-  </si>
-  <si>
     <t>SuiteName*</t>
   </si>
   <si>
@@ -198,10 +155,10 @@
     <t>Available</t>
   </si>
   <si>
-    <t>Suite-14:02:24</t>
-  </si>
-  <si>
-    <t>Suite-14:03:21</t>
+    <t>Suite-15:19:33</t>
+  </si>
+  <si>
+    <t>Suite-15:20:30</t>
   </si>
   <si>
     <t>Update SuiteName</t>
@@ -228,39 +185,18 @@
     <t>In-Active</t>
   </si>
   <si>
-    <t>Royal-14:05:07</t>
+    <t>Royal-15:22:39</t>
   </si>
   <si>
     <t>CreatedSuites</t>
   </si>
   <si>
-    <t>Suite-18:53:03</t>
-  </si>
-  <si>
-    <t>Royal-18:55:34</t>
-  </si>
-  <si>
-    <t>Suite-11:19:08</t>
-  </si>
-  <si>
-    <t>Suite-11:33:55</t>
-  </si>
-  <si>
-    <t>Royal-11:38:44</t>
-  </si>
-  <si>
     <t>Created SuiteName</t>
   </si>
   <si>
     <t>Updated SuiteName</t>
   </si>
   <si>
-    <t>Suite-18:53:49</t>
-  </si>
-  <si>
-    <t>Suite-11:34:48</t>
-  </si>
-  <si>
     <t>First Name*</t>
   </si>
   <si>
@@ -402,7 +338,7 @@
     <t>1234567890</t>
   </si>
   <si>
-    <t>David-06:04</t>
+    <t>David-24:59</t>
   </si>
   <si>
     <t>22</t>
@@ -417,7 +353,7 @@
     <t>1985</t>
   </si>
   <si>
-    <t>Johnson S David-06:04</t>
+    <t>Johnson S David-24:59</t>
   </si>
   <si>
     <t>female</t>
@@ -437,22 +373,16 @@
     </r>
   </si>
   <si>
-    <t>9805195939</t>
+    <t>9410283942</t>
   </si>
   <si>
     <t>notspecify</t>
   </si>
   <si>
-    <t>Created Suite Name</t>
-  </si>
-  <si>
-    <t>Created Ind Name</t>
+    <t>Selected Suites</t>
   </si>
   <si>
     <t>Individual ID</t>
-  </si>
-  <si>
-    <t>Emily S Martin-10:25</t>
   </si>
   <si>
     <t>Emily</t>
@@ -519,7 +449,10 @@
     <t>Others</t>
   </si>
   <si>
-    <t>Martin-10:25</t>
+    <t>Martin-44:45</t>
+  </si>
+  <si>
+    <t>Emily S Martin-44:45</t>
   </si>
   <si>
     <t>Male</t>
@@ -528,7 +461,7 @@
     <t>Royal-21:49:51</t>
   </si>
   <si>
-    <t>9203841740</t>
+    <t>9312494783</t>
   </si>
   <si>
     <t>Prefer not to say</t>
@@ -538,12 +471,6 @@
   </si>
   <si>
     <t>Updated IndividualNames</t>
-  </si>
-  <si>
-    <t>Johnson S David-47:09</t>
-  </si>
-  <si>
-    <t>Emily S Martin-53:09</t>
   </si>
   <si>
     <r>
@@ -876,13 +803,22 @@
     <t>Individual Name</t>
   </si>
   <si>
-    <t>Fall Description</t>
-  </si>
-  <si>
-    <t>Emily S Martin-10:25(Royal-14:05:07)</t>
-  </si>
-  <si>
-    <t>01/29/202406:41PM</t>
+    <t>Alert Notification Description</t>
+  </si>
+  <si>
+    <t>Staff Message</t>
+  </si>
+  <si>
+    <t>Chief Nurse Message</t>
+  </si>
+  <si>
+    <t>Manager Message</t>
+  </si>
+  <si>
+    <t>Johnson S David-24:59(Suite-15:19:33)</t>
+  </si>
+  <si>
+    <t>02/02/202401:24PM</t>
   </si>
   <si>
     <t>Low BP</t>
@@ -915,19 +851,19 @@
     <t>John Smith</t>
   </si>
   <si>
-    <t>1/29/2024</t>
-  </si>
-  <si>
-    <t>06:42PM</t>
+    <t>2/2/2024</t>
+  </si>
+  <si>
+    <t>01:24PM</t>
   </si>
   <si>
     <t>Jane Doe</t>
   </si>
   <si>
-    <t>Twisted Ankle-42:15</t>
-  </si>
-  <si>
-    <t>IR00240</t>
+    <t>Twisted Ankle-24:49</t>
+  </si>
+  <si>
+    <t>IR00361</t>
   </si>
   <si>
     <t>Chief nurse approved.</t>
@@ -954,46 +890,22 @@
     <t>Social Worker rejected.</t>
   </si>
   <si>
-    <t>Emily Martin-10:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Fall </t>
-  </si>
-  <si>
-    <t>Suite-17:00:45</t>
-  </si>
-  <si>
-    <t>Suite-17:01:34</t>
-  </si>
-  <si>
-    <t>Royal-17:02:54</t>
-  </si>
-  <si>
-    <t>Suite-17:07:28</t>
-  </si>
-  <si>
-    <t>Suite-17:08:17</t>
-  </si>
-  <si>
-    <t>Royal-17:10:20</t>
-  </si>
-  <si>
-    <t>David-11:21</t>
-  </si>
-  <si>
-    <t>Johnson S David-11:21</t>
-  </si>
-  <si>
-    <t>9843844755</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Johnson David-11:21</t>
-  </si>
-  <si>
-    <t>Johnson S David-11:21(Royal-17:10:20)</t>
+    <t>Johnson David-24:59</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Staff Test Message</t>
+  </si>
+  <si>
+    <t>Chief Nurse Test Message</t>
+  </si>
+  <si>
+    <t>Manager Test Message</t>
+  </si>
+  <si>
+    <t>Suite-13:04:03</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +919,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1033,12 +945,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00151D"/>
-      <name val="Comic Sans MS"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Comic Sans MS"/>
       <charset val="134"/>
     </font>
@@ -1109,25 +1015,6 @@
       <sz val="12"/>
       <color rgb="FF374151"/>
       <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="SF-Pro-Display-Regular"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1704,137 +1591,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1851,65 +1738,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1917,52 +1800,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2287,7 +2161,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -2297,34 +2171,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="54" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="53" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="54" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2342,72 +2216,17 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="19.2727272727273"/>
-    <col min="2" max="2" customWidth="true" width="20.6363636363636"/>
-    <col min="3" max="3" customWidth="true" width="11.1818181818182"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
     <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
-    <col min="7" max="7" customWidth="true" style="20" width="27.6363636363636"/>
+    <col min="7" max="7" customWidth="true" style="19" width="27.6363636363636"/>
     <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
     <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
     <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
@@ -2418,203 +2237,203 @@
     <col min="28" max="16383" customWidth="true" width="10.9090909090909"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="17" spans="1:27">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
+      <c r="A1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="W1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="X1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="Y1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="Z1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="AA1" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" ht="17.5" spans="1:27">
+      <c r="A2" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="C2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z1" s="13" t="s">
+      <c r="E2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" ht="17.5" spans="1:27">
-      <c r="A2" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="V2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="W2" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="X2" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="Y2" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="65" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="M2" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="U2" s="67" t="s">
-        <v>123</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="W2" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="X2" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y2" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z2" s="60" t="s">
-        <v>128</v>
-      </c>
       <c r="AA2" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>114</v>
+        <v>134</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G4" s="28"/>
+        <v>137</v>
+      </c>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="28"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="28"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -2635,7 +2454,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>6</v>
       </c>
       <c r="H8">
@@ -2700,130 +2519,159 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="28"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="28"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="28"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="28"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="28"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="28"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="28"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="28"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="28"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="28"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="28"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="28"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="28"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="28"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="28"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="28"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="28"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="28"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="28"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="28"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="28"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="28"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="28"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="28"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="28"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="28"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="28"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="28"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="28"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="28"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="28"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="28"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="28"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="28"/>
+      <c r="G42" s="27"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="28"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="28"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="28"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="28"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="28"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="28"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="28"/>
+      <c r="G49" s="27"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="28"/>
+      <c r="G50" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.6363636363636"/>
+    <col min="2" max="2" customWidth="true" width="29.2727272727273"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2832,51 +2680,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A2:B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="23.6363636363636"/>
-    <col min="2" max="2" customWidth="true" width="29.2727272727273"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H7"/>
@@ -2898,56 +2701,56 @@
     <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" spans="1:8">
-      <c r="A1" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>171</v>
+    <row r="1" s="10" customFormat="1" spans="1:8">
+      <c r="A1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="60" t="s">
-        <v>172</v>
+      <c r="A2" s="59" t="s">
+        <v>148</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="71" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="60" t="s">
-        <v>177</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="72" t="s">
-        <v>179</v>
+        <v>149</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2977,19 +2780,19 @@
       </c>
     </row>
     <row r="6" ht="17.5" spans="7:8">
-      <c r="G6" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>181</v>
+      <c r="G6" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
-      <c r="G7" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>183</v>
+      <c r="G7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2998,7 +2801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I7"/>
@@ -3020,62 +2823,62 @@
     <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" spans="1:9">
-      <c r="A1" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>184</v>
+    <row r="1" s="10" customFormat="1" spans="1:9">
+      <c r="A1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
       <c r="A2" s="6" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" s="71" t="s">
-        <v>188</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="F2" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="H2" s="73" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>168</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="9:9">
@@ -3108,19 +2911,19 @@
       </c>
     </row>
     <row r="6" ht="17.5" spans="7:8">
-      <c r="G6" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>181</v>
+      <c r="G6" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
-      <c r="G7" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>183</v>
+      <c r="G7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3129,18 +2932,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.0909090909091"/>
+    <col min="1" max="1" customWidth="true" width="32.1818181818182"/>
+    <col min="2" max="2" customWidth="true" width="20.0909090909091"/>
     <col min="3" max="3" customWidth="true" width="24.2727272727273"/>
     <col min="4" max="4" customWidth="true" width="20.0909090909091"/>
     <col min="5" max="5" customWidth="true" width="24.2727272727273"/>
@@ -3158,194 +2962,217 @@
     <col min="25" max="25" customWidth="true" width="44.8545454545455"/>
     <col min="26" max="27" customWidth="true" width="55.0"/>
     <col min="28" max="28" customWidth="true" width="46.7181818181818"/>
-    <col min="29" max="16384" customWidth="true" width="20.0909090909091"/>
+    <col min="29" max="29" customWidth="true" width="20.0909090909091"/>
+    <col min="30" max="30" customWidth="true" width="33.5727272727273"/>
+    <col min="31" max="31" customWidth="true" width="20.0909090909091"/>
+    <col min="32" max="32" customWidth="true" width="24.2818181818182"/>
+    <col min="33" max="33" customWidth="true" width="23.0"/>
+    <col min="34" max="16384" customWidth="true" width="20.0909090909091"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="17" spans="1:30">
+    <row r="1" s="1" customFormat="1" ht="17" spans="1:33">
       <c r="A1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="AA1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="AC1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="AD1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="AE1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="AF1" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="AG1" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="5" t="s">
+    </row>
+    <row r="2" ht="101.5" spans="1:33">
+      <c r="A2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="G2" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="H2" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="J2" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="K2" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="L2" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="M2" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="N2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="P2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Q2" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="R2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="T2" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="U2" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="V2" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="W2" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="X2" s="6" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="2" ht="101.5" spans="1:30">
-      <c r="A2" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="Y2" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z2" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="AD2" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="AE2" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="AG2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="1" spans="1:30">
+    </row>
+    <row r="11" s="2" customFormat="1" spans="1:33">
       <c r="A11" s="2">
         <v>0</v>
       </c>
@@ -3420,6 +3247,15 @@
       </c>
       <c r="AD11" s="2">
         <v>29</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>30</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>31</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3451,41 +3287,39 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
     <col min="2" max="2" customWidth="true" width="27.3636363636364"/>
-    <col min="3" max="3" customWidth="true" width="23.3636363636364"/>
+    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://xat.qa.xealei.com/" tooltip="https://xat.qa.xealei.com/"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://gha.qa.xealei.com/login"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3495,137 +3329,106 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.5454545454545"/>
+    <col min="1" max="1" customWidth="true" width="18.0"/>
     <col min="2" max="2" customWidth="true" width="34.0"/>
     <col min="3" max="16382" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="50" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="48" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="47" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="53" t="s">
+      <c r="B3" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="C3" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="B4" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="55" t="s">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="B5" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="53" t="s">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B6" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C6" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="47" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="53" t="s">
+      <c r="B7" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="54" t="s">
+      <c r="C7" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="D7" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3644,171 +3447,103 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.5454545454545"/>
-    <col min="2" max="2" customWidth="true" width="26.3636363636364"/>
-    <col min="3" max="3" customWidth="true" width="17.2727272727273"/>
-    <col min="4" max="4" customWidth="true" width="24.2727272727273"/>
-    <col min="5" max="5" customWidth="true" width="33.4545454545455"/>
+    <col min="1" max="1" customWidth="true" style="33" width="13.3636363636364"/>
+    <col min="2" max="2" customWidth="true" style="33" width="28.7272727272727"/>
+    <col min="3" max="5" customWidth="true" style="33" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
+    <col min="7" max="7" customWidth="true" width="16.8181818181818"/>
+    <col min="8" max="16381" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="50" t="s">
+    <row r="1" s="40" customFormat="1" ht="19.5" spans="1:7">
+      <c r="A1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="50" t="s">
+    </row>
+    <row r="2" ht="15.5" spans="1:7">
+      <c r="A2" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="B2" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D2" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="60" t="s">
+      <c r="E2" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="F2" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="60" t="s">
+      <c r="G2" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="7:7">
+      <c r="G3" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="61" t="s">
-        <v>44</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="33">
+        <v>0</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1</v>
+      </c>
+      <c r="C6" s="33">
+        <v>2</v>
+      </c>
+      <c r="D6" s="33">
+        <v>3</v>
+      </c>
+      <c r="E6" s="33">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mohamedrazul.s@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId2" display="123@g.in"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" style="37" width="12.6363636363636"/>
-    <col min="2" max="2" customWidth="true" style="37" width="28.7272727272727"/>
-    <col min="3" max="5" customWidth="true" style="37" width="12.6363636363636"/>
-    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
-    <col min="7" max="7" customWidth="true" width="16.8181818181818"/>
-    <col min="8" max="16381" customWidth="true" width="12.6363636363636"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="44" customFormat="1" ht="19.5" spans="1:7">
-      <c r="A1" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="7:7">
-      <c r="G3" s="6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="37">
-        <v>0</v>
-      </c>
-      <c r="B6" s="37">
-        <v>1</v>
-      </c>
-      <c r="C6" s="37">
-        <v>2</v>
-      </c>
-      <c r="D6" s="37">
-        <v>3</v>
-      </c>
-      <c r="E6" s="37">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G10"/>
@@ -3821,65 +3556,65 @@
   <cols>
     <col min="1" max="1" customWidth="true" width="21.7272727272727"/>
     <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
-    <col min="3" max="5" customWidth="true" style="37" width="12.9090909090909"/>
+    <col min="3" max="5" customWidth="true" style="33" width="12.9090909090909"/>
     <col min="6" max="6" customWidth="true" width="30.9090909090909"/>
     <col min="7" max="7" customWidth="true" width="22.2727272727273"/>
     <col min="8" max="16379" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
-      <c r="A1" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="38" t="s">
+    </row>
+    <row r="2" ht="15.5" spans="1:7">
+      <c r="A2" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="B2" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" ht="15.5" spans="1:7">
-      <c r="A2" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>64</v>
+      <c r="E2" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="37"/>
-      <c r="F3" s="43" t="s">
-        <v>65</v>
+      <c r="B3" s="33"/>
+      <c r="F3" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>256</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3889,13 +3624,13 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="33">
         <v>2</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="33">
         <v>3</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="33">
         <v>4</v>
       </c>
       <c r="F10">
@@ -3903,6 +3638,36 @@
       </c>
       <c r="G10">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3914,75 +3679,24 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.9090909090909"/>
+    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
+    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>256</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3994,86 +3708,17 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
-    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
     <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
-    <col min="7" max="7" customWidth="true" style="20" width="27.6363636363636"/>
+    <col min="7" max="7" customWidth="true" style="19" width="27.6363636363636"/>
     <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
     <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
     <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
@@ -4084,203 +3729,201 @@
     <col min="28" max="16384" customWidth="true" width="10.9090909090909"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="17" spans="1:27">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
+      <c r="A1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="W1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="X1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="Y1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="Z1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="AA1" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="C2" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="E2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="F2" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="G2" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="I2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="J2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="K2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="L2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="M2" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="N2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="O2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="P2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Q2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="R2" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="S2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="T2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="U2" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="V2" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="23" t="s">
+      <c r="W2" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="X2" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="Y2" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="Z2" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="F2" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="66" t="s">
-        <v>254</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="M2" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="U2" s="67" t="s">
-        <v>123</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="W2" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="X2" s="60" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y2" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z2" s="60" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="68" t="s">
-        <v>256</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>132</v>
+        <v>109</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="K3" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>111</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>259</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="G4" s="28"/>
+        <v>113</v>
+      </c>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="7:7">
-      <c r="G6" s="28"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="7:7">
-      <c r="G7" s="28"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8">
@@ -4301,7 +3944,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>6</v>
       </c>
       <c r="H8">
@@ -4366,130 +4009,163 @@
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="28"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="7:7">
-      <c r="G10" s="28"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="7:7">
-      <c r="G11" s="28"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="7:7">
-      <c r="G12" s="28"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="28"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="7:7">
-      <c r="G14" s="28"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="7:7">
-      <c r="G15" s="28"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="7:7">
-      <c r="G16" s="28"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="7:7">
-      <c r="G17" s="28"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="28"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="7:7">
-      <c r="G19" s="28"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="7:7">
-      <c r="G20" s="28"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="28"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="7:7">
-      <c r="G22" s="28"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="7:7">
-      <c r="G23" s="28"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="7:7">
-      <c r="G24" s="28"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="7:7">
-      <c r="G25" s="28"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="7:7">
-      <c r="G26" s="28"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="7:7">
-      <c r="G27" s="28"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="7:7">
-      <c r="G28" s="28"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="7:7">
-      <c r="G29" s="28"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="7:7">
-      <c r="G30" s="28"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="7:7">
-      <c r="G31" s="28"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="7:7">
-      <c r="G32" s="28"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="7:7">
-      <c r="G33" s="28"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="7:7">
-      <c r="G34" s="28"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="7:7">
-      <c r="G35" s="28"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="7:7">
-      <c r="G36" s="28"/>
+      <c r="G36" s="27"/>
     </row>
     <row r="37" spans="7:7">
-      <c r="G37" s="28"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="7:7">
-      <c r="G38" s="28"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="7:7">
-      <c r="G39" s="28"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="7:7">
-      <c r="G40" s="28"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="7:7">
-      <c r="G41" s="28"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" spans="7:7">
-      <c r="G42" s="28"/>
+      <c r="G42" s="27"/>
     </row>
     <row r="43" spans="7:7">
-      <c r="G43" s="28"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="7:7">
-      <c r="G44" s="28"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="7:7">
-      <c r="G45" s="28"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="7:7">
-      <c r="G46" s="28"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="7:7">
-      <c r="G47" s="28"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="7:7">
-      <c r="G48" s="28"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="7:7">
-      <c r="G49" s="28"/>
+      <c r="G49" s="27"/>
     </row>
     <row r="50" spans="7:7">
-      <c r="G50" s="28"/>
+      <c r="G50" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="19.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="20.6363636363636"/>
+    <col min="3" max="3" customWidth="true" width="11.1818181818182"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Reports Changes - Passed Scenario
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="7" activeTab="7"/>
+    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="416">
   <si>
     <t>Environment Name</t>
   </si>
@@ -410,7 +410,7 @@
     <t>1234567890</t>
   </si>
   <si>
-    <t>David-19:48</t>
+    <t>David-26:06</t>
   </si>
   <si>
     <t>22</t>
@@ -425,7 +425,7 @@
     <t>1985</t>
   </si>
   <si>
-    <t>Johnson S David-19:48</t>
+    <t>Johnson S David-26:06</t>
   </si>
   <si>
     <t>female</t>
@@ -448,7 +448,7 @@
     </r>
   </si>
   <si>
-    <t>9119479941</t>
+    <t>9593494525</t>
   </si>
   <si>
     <t>notspecify</t>
@@ -536,6 +536,18 @@
   </si>
   <si>
     <t>56</t>
+  </si>
+  <si>
+    <t>Johnson S David-24:52</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>Emily S Martin-57:17</t>
+  </si>
+  <si>
+    <t>59</t>
   </si>
   <si>
     <t>Emily</t>
@@ -602,10 +614,7 @@
     <t>Others</t>
   </si>
   <si>
-    <t>Martin-44:45</t>
-  </si>
-  <si>
-    <t>Emily S Martin-44:45</t>
+    <t>Martin-57:17</t>
   </si>
   <si>
     <t>Male</t>
@@ -614,7 +623,7 @@
     <t>Royal-21:49:51</t>
   </si>
   <si>
-    <t>9312494783</t>
+    <t>9614317168</t>
   </si>
   <si>
     <t>Prefer not to say</t>
@@ -624,6 +633,9 @@
   </si>
   <si>
     <t>Updated IndividualNames</t>
+  </si>
+  <si>
+    <t>Emily S Martin-50:12</t>
   </si>
   <si>
     <r>
@@ -968,7 +980,7 @@
     <t>Manager Message</t>
   </si>
   <si>
-    <t>Johnson S David-15:46(Suite-17:27:53)</t>
+    <t>Emily S Martin-27:12(Suite-10:37:23)</t>
   </si>
   <si>
     <t>02/02/202401:24PM</t>
@@ -1013,7 +1025,7 @@
     <t>Jane Doe</t>
   </si>
   <si>
-    <t>Twisted Ankle-24:49</t>
+    <t>Twisted Ankle-54:39</t>
   </si>
   <si>
     <t>IR00361</t>
@@ -1043,7 +1055,7 @@
     <t>Social Worker rejected.</t>
   </si>
   <si>
-    <t>Johnson David-15:46</t>
+    <t>Emily Martin-57:17</t>
   </si>
   <si>
     <t>test</t>
@@ -1058,55 +1070,388 @@
     <t>Manager Test Message</t>
   </si>
   <si>
-    <t>David-23:52</t>
-  </si>
-  <si>
-    <t>Johnson S David-23:52</t>
-  </si>
-  <si>
-    <t>9679326379</t>
-  </si>
-  <si>
-    <t>9041663469</t>
-  </si>
-  <si>
-    <t>9355756969</t>
-  </si>
-  <si>
-    <t>David-24:52</t>
-  </si>
-  <si>
-    <t>Johnson S David-24:52</t>
-  </si>
-  <si>
-    <t>9405240724</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>Johnson David-24:52</t>
-  </si>
-  <si>
-    <t>Johnson S David-24:52(Johnson S David-24:52)</t>
-  </si>
-  <si>
-    <t>David-26:06</t>
-  </si>
-  <si>
-    <t>Johnson S David-26:06</t>
-  </si>
-  <si>
-    <t>9593494525</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>Johnson David-26:06</t>
-  </si>
-  <si>
-    <t>Johnson S David-26:06(Suite-18:33:38)</t>
+    <t>Twisted Ankle-04:41</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-25:20</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-44:32</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-47:06</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-40:26</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-43:03</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-56:44</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-59:26</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-15:56</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-18:34</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-38:25</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-41:01</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-45:29</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-47:49</t>
+  </si>
+  <si>
+    <t>02/08/202410:54PM</t>
+  </si>
+  <si>
+    <t>02/08/202411:11PM</t>
+  </si>
+  <si>
+    <t>02/08/202411:13PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-14:06</t>
+  </si>
+  <si>
+    <t>2/8/2024</t>
+  </si>
+  <si>
+    <t>11:14PM</t>
+  </si>
+  <si>
+    <t>IR00374</t>
+  </si>
+  <si>
+    <t>02/08/202411:17PM</t>
+  </si>
+  <si>
+    <t>02/08/202411:22PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-22:53</t>
+  </si>
+  <si>
+    <t>11:22PM</t>
+  </si>
+  <si>
+    <t>IR00375</t>
+  </si>
+  <si>
+    <t>02/08/202411:26PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-27:13</t>
+  </si>
+  <si>
+    <t>11:27PM</t>
+  </si>
+  <si>
+    <t>IR00376</t>
+  </si>
+  <si>
+    <t>Suite-23:42:57</t>
+  </si>
+  <si>
+    <t>Suite-23:45:12</t>
+  </si>
+  <si>
+    <t>Royal-23:46:18</t>
+  </si>
+  <si>
+    <t>David-47:14</t>
+  </si>
+  <si>
+    <t>Johnson S David-47:14</t>
+  </si>
+  <si>
+    <t>9557112689</t>
+  </si>
+  <si>
+    <t>9645080841</t>
+  </si>
+  <si>
+    <t>9359513053</t>
+  </si>
+  <si>
+    <t>David-48:16</t>
+  </si>
+  <si>
+    <t>Johnson S David-48:16</t>
+  </si>
+  <si>
+    <t>9056212311</t>
+  </si>
+  <si>
+    <t>David-52:14</t>
+  </si>
+  <si>
+    <t>Johnson S David-52:14</t>
+  </si>
+  <si>
+    <t>9349193907</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Johnson David-52:14</t>
+  </si>
+  <si>
+    <t>Johnson S David-52:14(Royal-23:46:18)</t>
+  </si>
+  <si>
+    <t>Martin-55:34</t>
+  </si>
+  <si>
+    <t>9921287462</t>
+  </si>
+  <si>
+    <t>Emily S Martin-55:34</t>
+  </si>
+  <si>
+    <t>Emily Martin-55:34</t>
+  </si>
+  <si>
+    <t>Emily S Martin-55:34(Royal-23:46:18)</t>
+  </si>
+  <si>
+    <t>Suite-07:49:55</t>
+  </si>
+  <si>
+    <t>Suite-07:53:56</t>
+  </si>
+  <si>
+    <t>Suite-07:55:00</t>
+  </si>
+  <si>
+    <t>Suite-08:09:22</t>
+  </si>
+  <si>
+    <t>Suite-08:13:04</t>
+  </si>
+  <si>
+    <t>Suite-08:15:59</t>
+  </si>
+  <si>
+    <t>Suite-08:18:08</t>
+  </si>
+  <si>
+    <t>Suite-08:34:20</t>
+  </si>
+  <si>
+    <t>Suite-08:38:50</t>
+  </si>
+  <si>
+    <t>Suite-08:52:10</t>
+  </si>
+  <si>
+    <t>Royal-09:13:46</t>
+  </si>
+  <si>
+    <t>David-23:08</t>
+  </si>
+  <si>
+    <t>Johnson S David-23:08</t>
+  </si>
+  <si>
+    <t>9907326634</t>
+  </si>
+  <si>
+    <t>9555558788</t>
+  </si>
+  <si>
+    <t>9867715895</t>
+  </si>
+  <si>
+    <t>David-24:05</t>
+  </si>
+  <si>
+    <t>Johnson S David-24:05</t>
+  </si>
+  <si>
+    <t>9190233040</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>Johnson David-24:05</t>
+  </si>
+  <si>
+    <t>Johnson S David-24:05(Johnson S David-24:05)</t>
+  </si>
+  <si>
+    <t>David-25:06</t>
+  </si>
+  <si>
+    <t>Johnson S David-25:06</t>
+  </si>
+  <si>
+    <t>9484788180</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>Johnson David-25:06</t>
+  </si>
+  <si>
+    <t>Johnson S David-25:06(Royal-09:13:46)</t>
+  </si>
+  <si>
+    <t>02/09/202411:16AM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-17:29</t>
+  </si>
+  <si>
+    <t>2/9/2024</t>
+  </si>
+  <si>
+    <t>11:17AM</t>
+  </si>
+  <si>
+    <t>IR00377</t>
+  </si>
+  <si>
+    <t>02/09/202411:21AM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-22:19</t>
+  </si>
+  <si>
+    <t>11:22AM</t>
+  </si>
+  <si>
+    <t>IR00378</t>
+  </si>
+  <si>
+    <t>02/09/202411:27AM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-28:18</t>
+  </si>
+  <si>
+    <t>11:28AM</t>
+  </si>
+  <si>
+    <t>IR00379</t>
+  </si>
+  <si>
+    <t>02/09/202411:36AM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-36:42</t>
+  </si>
+  <si>
+    <t>11:36AM</t>
+  </si>
+  <si>
+    <t>IR00380</t>
+  </si>
+  <si>
+    <t>02/09/202411:41AM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-41:54</t>
+  </si>
+  <si>
+    <t>11:41AM</t>
+  </si>
+  <si>
+    <t>IR00381</t>
+  </si>
+  <si>
+    <t>02/09/202411:44AM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-45:28</t>
+  </si>
+  <si>
+    <t>11:45AM</t>
+  </si>
+  <si>
+    <t>IR00382</t>
+  </si>
+  <si>
+    <t>02/09/202412:37PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-37:10</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-37:51</t>
+  </si>
+  <si>
+    <t>02/09/202412:38PM</t>
+  </si>
+  <si>
+    <t>02/09/202412:41PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-41:28</t>
+  </si>
+  <si>
+    <t>02/09/202412:42PM</t>
+  </si>
+  <si>
+    <t>12:43PM</t>
+  </si>
+  <si>
+    <t>02/09/202412:43PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-44:07</t>
+  </si>
+  <si>
+    <t>12:44PM</t>
+  </si>
+  <si>
+    <t>02/09/202412:45PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-45:38</t>
+  </si>
+  <si>
+    <t>12:45PM</t>
+  </si>
+  <si>
+    <t>IR00386</t>
+  </si>
+  <si>
+    <t>02/09/202412:49PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-49:51</t>
+  </si>
+  <si>
+    <t>12:49PM</t>
+  </si>
+  <si>
+    <t>IR00387</t>
+  </si>
+  <si>
+    <t>02/09/202412:52PM</t>
+  </si>
+  <si>
+    <t>Twisted Ankle-53:08</t>
+  </si>
+  <si>
+    <t>12:53PM</t>
+  </si>
+  <si>
+    <t>IR00388</t>
   </si>
 </sst>
 </file>
@@ -1922,7 +2267,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1931,13 +2276,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2040,6 +2385,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2524,34 +2872,34 @@
     </row>
     <row r="2" ht="17.5" spans="1:27">
       <c r="A2" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>107</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>169</v>
+      <c r="E2" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>135</v>
@@ -2560,34 +2908,34 @@
         <v>136</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" s="6" t="s">
         <v>179</v>
       </c>
+      <c r="N2" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="R2" s="31" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="U2" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>183</v>
+      <c r="V2" s="8" t="s">
+        <v>335</v>
       </c>
       <c r="W2" s="59" t="s">
         <v>128</v>
@@ -2601,16 +2949,16 @@
       <c r="Z2" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" s="6" t="s">
-        <v>184</v>
+      <c r="AA2" s="8" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="5:21">
-      <c r="E3" s="6" t="s">
-        <v>185</v>
+      <c r="E3" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="K3" s="30" t="s">
         <v>116</v>
@@ -2618,13 +2966,13 @@
       <c r="L3" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>187</v>
+      <c r="U3" s="8" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="5:7">
-      <c r="E4" s="6" t="s">
-        <v>188</v>
+      <c r="E4" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="G4" s="27"/>
     </row>
@@ -2855,13 +3203,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="23.6363636363636"/>
     <col min="2" max="2" customWidth="true" width="29.2727272727273"/>
@@ -2869,10 +3217,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2905,54 +3277,54 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:8">
       <c r="A1" s="11" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
       <c r="A2" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>204</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H2" s="62" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2983,18 +3355,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3027,64 +3399,64 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:9">
       <c r="A1" s="11" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
-      <c r="A2" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>213</v>
+      <c r="A2" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>217</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H2" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="9:9">
-      <c r="I3" s="6"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
@@ -3114,18 +3486,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3139,8 +3511,8 @@
   <sheetPr/>
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5"/>
@@ -3174,204 +3546,204 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17" spans="1:33">
       <c r="A1" s="3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" ht="101.5" spans="1:33">
-      <c r="A2" s="6" t="s">
-        <v>300</v>
+      <c r="A2" s="64" t="s">
+        <v>367</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="G2" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="H2" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>125</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="R2" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="Y2" s="6" t="s">
+      <c r="S2" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="U2" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="V2" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="W2" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="X2" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="AC2" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="AD2" s="6" t="s">
+      <c r="Y2" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z2" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AA2" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AB2" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="AG2" s="6" t="s">
-        <v>283</v>
+      <c r="AC2" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:33">
@@ -3517,7 +3889,7 @@
       <c r="B2" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3568,7 +3940,7 @@
       <c r="C2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3582,7 +3954,7 @@
       <c r="C3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="48" t="s">
@@ -3594,7 +3966,7 @@
       <c r="C4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="48" t="s">
@@ -3606,7 +3978,7 @@
       <c r="C5" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="48" t="s">
@@ -3618,7 +3990,7 @@
       <c r="C6" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="48" t="s">
@@ -3630,7 +4002,7 @@
       <c r="C7" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3707,13 +4079,13 @@
       <c r="F2" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>42</v>
+      <c r="G2" s="8" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="7:7">
-      <c r="G3" s="6" t="s">
-        <v>43</v>
+      <c r="G3" s="8" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3806,8 +4178,8 @@
       <c r="F2" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>42</v>
+      <c r="G2" s="8" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="2:7">
@@ -3815,8 +4187,8 @@
       <c r="F3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>52</v>
+      <c r="G3" s="8" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3851,7 +4223,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A9"/>
@@ -3922,6 +4294,66 @@
         <v>52</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>350</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3931,7 +4363,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B4"/>
@@ -4050,6 +4482,22 @@
         <v>52</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B18" t="s">
+        <v>350</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -4061,7 +4509,7 @@
   <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4167,31 +4615,31 @@
       <c r="A2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>107</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F2" s="58" t="s">
         <v>111</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>112</v>
+        <v>346</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="8" t="s">
         <v>115</v>
       </c>
       <c r="K2" s="30" t="s">
@@ -4203,32 +4651,32 @@
       <c r="M2" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="8" t="s">
         <v>122</v>
       </c>
       <c r="R2" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="8" t="s">
         <v>125</v>
       </c>
       <c r="U2" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>295</v>
+      <c r="V2" s="8" t="s">
+        <v>362</v>
       </c>
       <c r="W2" s="59" t="s">
         <v>128</v>
@@ -4242,16 +4690,16 @@
       <c r="Z2" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" s="6" t="s">
-        <v>296</v>
+      <c r="AA2" s="8" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="5:21">
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>133</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>134</v>
+        <v>350</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>135</v>
@@ -4259,12 +4707,12 @@
       <c r="L3" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>297</v>
+      <c r="U3" s="8" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="5:7">
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>138</v>
       </c>
       <c r="G4" s="32"/>
@@ -4496,7 +4944,7 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -4640,23 +5088,53 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>290</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>296</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
-        <v>298</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" t="s">
+        <v>337</v>
+      </c>
+      <c r="C25" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>357</v>
+      </c>
+      <c r="C26" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>350</v>
+      </c>
+      <c r="B27" t="s">
+        <v>363</v>
+      </c>
+      <c r="C27" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Facility Admin Changes
</commit_message>
<xml_diff>
--- a/Excel/Test Datas.xlsx
+++ b/Excel/Test Datas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" firstSheet="12" activeTab="16"/>
+    <workbookView windowWidth="18350" windowHeight="6950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="266">
   <si>
     <t>Environment Name</t>
   </si>
@@ -88,61 +88,64 @@
     <t>FACILITY ADMIN</t>
   </si>
   <si>
+    <t>mohamedra01</t>
+  </si>
+  <si>
+    <t>auto@123</t>
+  </si>
+  <si>
+    <t>Xealei Automation Testing</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>AStaff01</t>
+  </si>
+  <si>
+    <t>CHIEF NURSE</t>
+  </si>
+  <si>
+    <t>AChiefNur02</t>
+  </si>
+  <si>
+    <t>RESIDENT MANAGER</t>
+  </si>
+  <si>
+    <t>AResident02</t>
+  </si>
+  <si>
+    <t>CLINICAL COORDINATOR</t>
+  </si>
+  <si>
+    <t>AClinical02</t>
+  </si>
+  <si>
+    <t>SOCIAL WORKER</t>
+  </si>
+  <si>
+    <t>ASocialWo02</t>
+  </si>
+  <si>
+    <t>Unsupported format Mail Id</t>
+  </si>
+  <si>
+    <t>Mail Body Content</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Invalid Data</t>
+  </si>
+  <si>
     <t>mohamedra</t>
   </si>
   <si>
-    <t>auto@123</t>
-  </si>
-  <si>
-    <t>Automation Testing</t>
-  </si>
-  <si>
-    <t>STAFF</t>
-  </si>
-  <si>
-    <t>AStaff</t>
-  </si>
-  <si>
-    <t>CHIEF NURSE</t>
-  </si>
-  <si>
-    <t>AChiefNur</t>
-  </si>
-  <si>
-    <t>RESIDENT MANAGER</t>
-  </si>
-  <si>
-    <t>AResident</t>
-  </si>
-  <si>
-    <t>CLINICAL COORDINATOR</t>
-  </si>
-  <si>
-    <t>AClinical</t>
-  </si>
-  <si>
-    <t>SOCIAL WORKER</t>
-  </si>
-  <si>
-    <t>ASocialWo</t>
-  </si>
-  <si>
-    <t>Unsupported format Mail Id</t>
-  </si>
-  <si>
-    <t>Mail Body Content</t>
-  </si>
-  <si>
-    <t>New Password</t>
-  </si>
-  <si>
-    <t>Invalid Data</t>
-  </si>
-  <si>
-    <t>xealeiauto@mailinator.com</t>
-  </si>
-  <si>
-    <t>MTesting</t>
+    <t>autoxealei@mailinator.com</t>
+  </si>
+  <si>
+    <t>MTesting01</t>
   </si>
   <si>
     <t>Welcome to
@@ -158,13 +161,13 @@
     <t>mohamedra@13</t>
   </si>
   <si>
-    <t>Hi MTesting,</t>
+    <t>Hi MTesting01,</t>
   </si>
   <si>
     <t>mohamedrazul.s+100@alphind.com</t>
   </si>
   <si>
-    <t>You recently requested a password reset for your Xealei account xealeiauto@mailinator.com. To complete the process, click the button/link below:</t>
+    <t>You recently requested a password reset for your Xealei account autoxealei@mailinator.com. To complete the process, click the button/link below:</t>
   </si>
   <si>
     <r>
@@ -1012,6 +1015,15 @@
   </si>
   <si>
     <t>No fall detected.</t>
+  </si>
+  <si>
+    <t>Suite-16:29:59</t>
+  </si>
+  <si>
+    <t>Suite-16:31:15</t>
+  </si>
+  <si>
+    <t>Suite-16:34:59</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1857,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1954,6 +1966,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2318,41 +2333,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="38.4545454545455" customWidth="1"/>
-    <col min="3" max="3" width="26.3636363636364" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.0"/>
+    <col min="2" max="2" customWidth="true" width="38.4545454545455"/>
+    <col min="3" max="3" customWidth="true" width="26.3636363636364"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="63"/>
+      <c r="D2" s="64"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2378,13 +2393,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="20.4545454545455" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.7272727272727"/>
+    <col min="2" max="2" customWidth="true" width="20.4545454545455"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2404,16 +2419,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="18.0909090909091" customWidth="1"/>
-    <col min="2" max="2" width="22.4545454545455" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0909090909091"/>
+    <col min="2" max="2" customWidth="true" width="22.4545454545455"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2433,16 +2448,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="27.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="30.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="30.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2456,208 +2471,210 @@
   <sheetPr/>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
-    <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
-    <col min="7" max="7" width="27.6363636363636" style="19" customWidth="1"/>
-    <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
-    <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
-    <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
-    <col min="24" max="24" width="19.7272727272727" customWidth="1"/>
-    <col min="25" max="25" width="21.6363636363636" customWidth="1"/>
-    <col min="26" max="26" width="18.9090909090909" customWidth="1"/>
-    <col min="27" max="27" width="20.5454545454545" customWidth="1"/>
-    <col min="28" max="16384" width="10.9090909090909" customWidth="1"/>
+    <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
+    <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
+    <col min="7" max="7" customWidth="true" style="19" width="27.6363636363636"/>
+    <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
+    <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
+    <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
+    <col min="24" max="24" customWidth="true" width="19.7272727272727"/>
+    <col min="25" max="25" customWidth="true" width="21.6363636363636"/>
+    <col min="26" max="26" customWidth="true" width="18.9090909090909"/>
+    <col min="27" max="27" customWidth="true" width="20.5454545454545"/>
+    <col min="28" max="16384" customWidth="true" width="10.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="67" t="s">
         <v>114</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>115</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="U2" s="68" t="s">
         <v>128</v>
       </c>
+      <c r="U2" s="69" t="s">
+        <v>129</v>
+      </c>
       <c r="V2" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="W2" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="X2" s="64" t="s">
+      <c r="W2" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="Y2" s="64" t="s">
+      <c r="X2" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="Z2" s="64" t="s">
+      <c r="Y2" s="65" t="s">
         <v>133</v>
       </c>
+      <c r="Z2" s="65" t="s">
+        <v>134</v>
+      </c>
       <c r="AA2" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>265</v>
+      </c>
       <c r="K3" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G4" s="31"/>
     </row>
@@ -2896,20 +2913,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="19.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="20.6363636363636" customWidth="1"/>
-    <col min="3" max="3" width="11.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="20.6363636363636"/>
+    <col min="3" max="3" customWidth="true" width="11.1818181818182"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2929,201 +2946,201 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="5" width="21.3636363636364" customWidth="1"/>
-    <col min="6" max="6" width="11.4545454545455" customWidth="1"/>
-    <col min="7" max="7" width="27.6363636363636" style="19" customWidth="1"/>
-    <col min="8" max="8" width="9.36363636363636" customWidth="1"/>
-    <col min="9" max="22" width="21.3636363636364" customWidth="1"/>
-    <col min="23" max="23" width="16.4545454545455" customWidth="1"/>
-    <col min="24" max="24" width="19.7272727272727" customWidth="1"/>
-    <col min="25" max="25" width="21.6363636363636" customWidth="1"/>
-    <col min="26" max="26" width="18.9090909090909" customWidth="1"/>
-    <col min="27" max="27" width="34.2727272727273" customWidth="1"/>
-    <col min="28" max="16382" width="10.9090909090909" customWidth="1"/>
+    <col min="1" max="5" customWidth="true" width="21.3636363636364"/>
+    <col min="6" max="6" customWidth="true" width="11.4545454545455"/>
+    <col min="7" max="7" customWidth="true" style="19" width="27.6363636363636"/>
+    <col min="8" max="8" customWidth="true" width="9.36363636363636"/>
+    <col min="9" max="22" customWidth="true" width="21.3636363636364"/>
+    <col min="23" max="23" customWidth="true" width="16.4545454545455"/>
+    <col min="24" max="24" customWidth="true" width="19.7272727272727"/>
+    <col min="25" max="25" customWidth="true" width="21.6363636363636"/>
+    <col min="26" max="26" customWidth="true" width="18.9090909090909"/>
+    <col min="27" max="27" customWidth="true" width="34.2727272727273"/>
+    <col min="28" max="16382" customWidth="true" width="10.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="1" ht="17" spans="1:27">
       <c r="A1" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" ht="17.5" spans="1:27">
       <c r="A2" s="22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="69" t="s">
         <v>146</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>147</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="S2" s="30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="U2" s="68" t="s">
-        <v>128</v>
+        <v>158</v>
+      </c>
+      <c r="U2" s="69" t="s">
+        <v>129</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="W2" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="X2" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="W2" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="Y2" s="64" t="s">
+      <c r="X2" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="Z2" s="64" t="s">
+      <c r="Y2" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="AA2" s="64" t="s">
-        <v>159</v>
+      <c r="Z2" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA2" s="65" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="5:21">
       <c r="E3" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G3" s="8"/>
       <c r="K3" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="5:7">
       <c r="E4" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G4" s="26"/>
     </row>
@@ -3362,16 +3379,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="23.6363636363636" customWidth="1"/>
-    <col min="2" max="2" width="29.2727272727273" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.6363636363636"/>
+    <col min="2" max="2" customWidth="true" width="29.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3385,73 +3402,73 @@
   <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="23.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="21.3636363636364" customWidth="1"/>
-    <col min="4" max="4" width="19.1818181818182" customWidth="1"/>
-    <col min="5" max="5" width="12.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="12.0909090909091" customWidth="1"/>
-    <col min="7" max="7" width="12.1818181818182" customWidth="1"/>
-    <col min="8" max="8" width="46.0909090909091" customWidth="1"/>
-    <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="23.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="21.3636363636364"/>
+    <col min="4" max="4" customWidth="true" width="19.1818181818182"/>
+    <col min="5" max="5" customWidth="true" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="12.0909090909091"/>
+    <col min="7" max="7" customWidth="true" width="12.1818181818182"/>
+    <col min="8" max="8" customWidth="true" width="46.0909090909091"/>
+    <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:8">
       <c r="A1" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="64" t="s">
-        <v>173</v>
+      <c r="A2" s="65" t="s">
+        <v>174</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="C2" s="65" t="s">
         <v>176</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="D2" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="65" t="s">
         <v>178</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="H2" s="71" t="s">
+      <c r="G2" s="65" t="s">
         <v>180</v>
+      </c>
+      <c r="H2" s="72" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3482,18 +3499,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3513,73 +3530,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.1818181818182" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="23.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="21.3636363636364" customWidth="1"/>
-    <col min="4" max="4" width="19.1818181818182" customWidth="1"/>
-    <col min="5" max="5" width="12.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="12.0909090909091" customWidth="1"/>
-    <col min="7" max="7" width="12.1818181818182" customWidth="1"/>
-    <col min="8" max="8" width="46.0909090909091" customWidth="1"/>
-    <col min="9" max="16384" width="19.1818181818182" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="23.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="21.3636363636364"/>
+    <col min="4" max="4" customWidth="true" width="19.1818181818182"/>
+    <col min="5" max="5" customWidth="true" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="12.0909090909091"/>
+    <col min="7" max="7" customWidth="true" width="12.1818181818182"/>
+    <col min="8" max="8" customWidth="true" width="46.0909090909091"/>
+    <col min="9" max="16384" customWidth="true" width="19.1818181818182"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:9">
       <c r="A1" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:9">
       <c r="A2" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="C2" s="65" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="D2" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="65" t="s">
         <v>191</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>192</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="G2" s="65" t="s">
         <v>193</v>
       </c>
+      <c r="H2" s="73" t="s">
+        <v>194</v>
+      </c>
       <c r="I2" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="9:9">
@@ -3613,18 +3630,18 @@
     </row>
     <row r="6" ht="17.5" spans="7:8">
       <c r="G6" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" ht="17.5" spans="7:8">
       <c r="G7" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3644,245 +3661,245 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.0909090909091" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.6363636363636" customWidth="1"/>
-    <col min="2" max="2" width="20.0909090909091" customWidth="1"/>
-    <col min="3" max="3" width="24.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="20.0909090909091" customWidth="1"/>
-    <col min="5" max="5" width="24.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="25.5454545454545" customWidth="1"/>
-    <col min="7" max="7" width="25.2727272727273" customWidth="1"/>
-    <col min="8" max="9" width="20.0909090909091" customWidth="1"/>
-    <col min="10" max="10" width="30.6363636363636" customWidth="1"/>
-    <col min="11" max="11" width="18.5454545454545" customWidth="1"/>
-    <col min="12" max="18" width="20.0909090909091" customWidth="1"/>
-    <col min="19" max="19" width="26.4272727272727" customWidth="1"/>
-    <col min="20" max="20" width="22.1454545454545" customWidth="1"/>
-    <col min="21" max="21" width="47.1454545454545" customWidth="1"/>
-    <col min="22" max="23" width="54.7181818181818" customWidth="1"/>
-    <col min="24" max="24" width="47.1454545454545" customWidth="1"/>
-    <col min="25" max="25" width="44.8545454545455" customWidth="1"/>
-    <col min="26" max="27" width="55" customWidth="1"/>
-    <col min="28" max="28" width="46.7181818181818" customWidth="1"/>
-    <col min="29" max="29" width="20.0909090909091" customWidth="1"/>
-    <col min="30" max="30" width="33.5727272727273" customWidth="1"/>
-    <col min="31" max="31" width="20.0909090909091" customWidth="1"/>
-    <col min="32" max="32" width="24.2818181818182" customWidth="1"/>
-    <col min="33" max="33" width="23" customWidth="1"/>
-    <col min="34" max="16384" width="20.0909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.6363636363636"/>
+    <col min="2" max="2" customWidth="true" width="20.0909090909091"/>
+    <col min="3" max="3" customWidth="true" width="24.2727272727273"/>
+    <col min="4" max="4" customWidth="true" width="20.0909090909091"/>
+    <col min="5" max="5" customWidth="true" width="24.2727272727273"/>
+    <col min="6" max="6" customWidth="true" width="25.5454545454545"/>
+    <col min="7" max="7" customWidth="true" width="25.2727272727273"/>
+    <col min="8" max="9" customWidth="true" width="20.0909090909091"/>
+    <col min="10" max="10" customWidth="true" width="30.6363636363636"/>
+    <col min="11" max="11" customWidth="true" width="18.5454545454545"/>
+    <col min="12" max="18" customWidth="true" width="20.0909090909091"/>
+    <col min="19" max="19" customWidth="true" width="26.4272727272727"/>
+    <col min="20" max="20" customWidth="true" width="22.1454545454545"/>
+    <col min="21" max="21" customWidth="true" width="47.1454545454545"/>
+    <col min="22" max="23" customWidth="true" width="54.7181818181818"/>
+    <col min="24" max="24" customWidth="true" width="47.1454545454545"/>
+    <col min="25" max="25" customWidth="true" width="44.8545454545455"/>
+    <col min="26" max="27" customWidth="true" width="55.0"/>
+    <col min="28" max="28" customWidth="true" width="46.7181818181818"/>
+    <col min="29" max="29" customWidth="true" width="20.0909090909091"/>
+    <col min="30" max="30" customWidth="true" width="33.5727272727273"/>
+    <col min="31" max="31" customWidth="true" width="20.0909090909091"/>
+    <col min="32" max="32" customWidth="true" width="24.2818181818182"/>
+    <col min="33" max="33" customWidth="true" width="23.0"/>
+    <col min="34" max="16384" customWidth="true" width="20.0909090909091"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17" spans="1:35">
       <c r="A1" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" ht="101.5" spans="1:35">
       <c r="A2" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>234</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AG2" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:35">
@@ -4014,9 +4031,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="31.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="27.3636363636364" customWidth="1"/>
-    <col min="3" max="3" width="14.2727272727273" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="27.3636363636364"/>
+    <col min="3" max="3" customWidth="true" width="14.2727272727273"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4031,7 +4048,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="52" t="s">
@@ -4053,15 +4070,17 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="21.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="16382" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.1818181818182"/>
+    <col min="2" max="2" customWidth="true" width="34.0"/>
+    <col min="3" max="3" customWidth="true" width="18.0"/>
+    <col min="4" max="4" customWidth="true" width="29.0"/>
+    <col min="5" max="16382" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4082,10 +4101,10 @@
       <c r="A2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -4096,10 +4115,10 @@
       <c r="A3" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="8"/>
@@ -4108,10 +4127,10 @@
       <c r="A4" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="8"/>
@@ -4120,10 +4139,10 @@
       <c r="A5" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="8"/>
@@ -4132,10 +4151,10 @@
       <c r="A6" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8"/>
@@ -4144,10 +4163,10 @@
       <c r="A7" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="8"/>
@@ -4172,18 +4191,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="37.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="31.1818181818182" customWidth="1"/>
-    <col min="3" max="3" width="14.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="20.8181818181818" customWidth="1"/>
-    <col min="5" max="5" width="53.3636363636364" style="47" customWidth="1"/>
-    <col min="6" max="6" width="16.0909090909091" customWidth="1"/>
-    <col min="7" max="16381" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.2727272727273"/>
+    <col min="2" max="2" customWidth="true" width="31.1818181818182"/>
+    <col min="3" max="3" customWidth="true" width="14.1818181818182"/>
+    <col min="4" max="4" customWidth="true" width="20.8181818181818"/>
+    <col min="5" max="5" customWidth="true" style="47" width="53.3636363636364"/>
+    <col min="6" max="6" customWidth="true" width="16.0909090909091"/>
+    <col min="7" max="16381" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" spans="1:7">
@@ -4211,63 +4230,63 @@
     </row>
     <row r="2" ht="29" spans="1:7">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="50" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="64" t="s">
         <v>39</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
       <c r="E3" s="55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="54" customHeight="1" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="53"/>
       <c r="C4" s="31"/>
       <c r="D4" s="54"/>
       <c r="E4" s="56" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" s="56" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" ht="39" customHeight="1" spans="5:5">
       <c r="E6" s="56" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="auto@123"/>
-    <hyperlink ref="B2" r:id="rId2" display="xealeiauto@mailinator.com" tooltip="mailto:xealeiauto@mailinator.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="autoxealei@mailinator.com" tooltip="mailto:autoxealei@mailinator.com"/>
     <hyperlink ref="F2" r:id="rId3" display="auto@12345"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4280,80 +4299,84 @@
   <sheetPr/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.3636363636364" style="33" customWidth="1"/>
-    <col min="2" max="2" width="22" style="33" customWidth="1"/>
-    <col min="3" max="5" width="12.6363636363636" style="33" customWidth="1"/>
-    <col min="6" max="6" width="20.2727272727273" customWidth="1"/>
-    <col min="7" max="7" width="16.8181818181818" customWidth="1"/>
-    <col min="8" max="8" width="50.2727272727273" customWidth="1"/>
-    <col min="9" max="16381" width="12.6363636363636" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="33" width="13.3636363636364"/>
+    <col min="2" max="2" customWidth="true" style="33" width="25.9090909090909"/>
+    <col min="3" max="5" customWidth="true" style="33" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="20.2727272727273"/>
+    <col min="7" max="7" customWidth="true" width="16.8181818181818"/>
+    <col min="8" max="8" customWidth="true" width="50.2727272727273"/>
+    <col min="9" max="16381" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
     <row r="1" s="40" customFormat="1" ht="19.5" spans="1:8">
       <c r="A1" s="34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" ht="15.5" spans="1:8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" ht="31" spans="1:8">
       <c r="A2" s="43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="D2" s="66" t="s">
         <v>56</v>
       </c>
+      <c r="E2" s="66" t="s">
+        <v>57</v>
+      </c>
       <c r="F2" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="64" t="s">
         <v>58</v>
       </c>
+      <c r="G2" s="45" t="s">
+        <v>264</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="7:8">
-      <c r="G3" s="45"/>
-      <c r="H3" s="64" t="s">
-        <v>59</v>
+      <c r="G3" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" s="65" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="8:8">
-      <c r="H4" s="64" t="s">
-        <v>60</v>
+      <c r="H4" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4391,69 +4414,71 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="21.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="12.9090909090909" style="33" customWidth="1"/>
-    <col min="6" max="6" width="30.9090909090909" customWidth="1"/>
-    <col min="7" max="7" width="22.2727272727273" customWidth="1"/>
-    <col min="8" max="16378" width="12.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7272727272727"/>
+    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
+    <col min="3" max="5" customWidth="true" style="33" width="12.9090909090909"/>
+    <col min="6" max="6" customWidth="true" width="30.9090909090909"/>
+    <col min="7" max="7" customWidth="true" width="22.2727272727273"/>
+    <col min="8" max="16378" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="37" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="66" t="s">
+      <c r="C2" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="67" t="s">
         <v>66</v>
       </c>
+      <c r="E2" s="67" t="s">
+        <v>67</v>
+      </c>
       <c r="F2" s="37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="8"/>
+        <v>69</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
@@ -4489,61 +4514,61 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6363636363636" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="25.0909090909091" style="33" customWidth="1"/>
-    <col min="2" max="2" width="22" style="33" customWidth="1"/>
-    <col min="3" max="5" width="12.6363636363636" style="33" customWidth="1"/>
-    <col min="6" max="6" width="28.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="30.3636363636364" customWidth="1"/>
-    <col min="8" max="16380" width="12.6363636363636" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="33" width="25.0909090909091"/>
+    <col min="2" max="2" customWidth="true" style="33" width="27.1818181818182"/>
+    <col min="3" max="5" customWidth="true" style="33" width="12.6363636363636"/>
+    <col min="6" max="6" customWidth="true" width="28.8181818181818"/>
+    <col min="7" max="7" customWidth="true" width="30.3636363636364"/>
+    <col min="8" max="16380" customWidth="true" width="12.6363636363636"/>
   </cols>
   <sheetData>
     <row r="1" s="40" customFormat="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" ht="15.5" spans="1:7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" ht="31" spans="1:7">
       <c r="A2" s="43" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="D2" s="66" t="s">
         <v>56</v>
       </c>
+      <c r="E2" s="66" t="s">
+        <v>57</v>
+      </c>
       <c r="F2" s="45" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G2" s="8"/>
     </row>
@@ -4584,68 +4609,68 @@
   <sheetPr/>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.9090909090909" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="32.8181818181818" customWidth="1"/>
-    <col min="2" max="2" width="32.3636363636364" customWidth="1"/>
-    <col min="3" max="5" width="12.9090909090909" style="33" customWidth="1"/>
-    <col min="6" max="6" width="36.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="33.2727272727273" customWidth="1"/>
-    <col min="8" max="16378" width="12.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.8181818181818"/>
+    <col min="2" max="2" customWidth="true" width="32.3636363636364"/>
+    <col min="3" max="5" customWidth="true" style="33" width="12.9090909090909"/>
+    <col min="6" max="6" customWidth="true" width="36.8181818181818"/>
+    <col min="7" max="7" customWidth="true" width="33.2727272727273"/>
+    <col min="8" max="16378" customWidth="true" width="12.9090909090909"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:7">
       <c r="A1" s="34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="66" t="s">
+      <c r="C2" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="67" t="s">
         <v>66</v>
       </c>
+      <c r="E2" s="67" t="s">
+        <v>67</v>
+      </c>
       <c r="F2" s="37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="33"/>
       <c r="F3" s="39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G3" s="8"/>
     </row>
@@ -4681,7 +4706,7 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A17"/>
@@ -4689,13 +4714,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.1818181818182" customWidth="1"/>
-    <col min="2" max="2" width="20.4545454545455" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.1818181818182"/>
+    <col min="2" max="2" customWidth="true" width="20.4545454545455"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>